<commit_message>
Add more tests and fix found bugs
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/BulgeChaserTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/BulgeChaserTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="-240" yWindow="1605" windowWidth="19440" windowHeight="11040" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="By Diag 6x6" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="31">
   <si>
     <t>#1</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>G[2-1]*A=</t>
+  </si>
+  <si>
+    <t>#5</t>
   </si>
 </sst>
 </file>
@@ -472,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM44"/>
+  <dimension ref="A1:AM53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:K7"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,17 +1224,17 @@
         <v>0</v>
       </c>
       <c r="AA12" s="1">
-        <f t="array" ref="AA12:AF17">MMULT(T12:Y17,MMULT(M12:R17,A12:F17))</f>
+        <f t="array" ref="AA12:AF17">MMULT(T12:Y17,MMULT(M12:R17,AH3:AM8))</f>
         <v>5.9958782371607278</v>
       </c>
       <c r="AB12" s="1">
-        <v>4.4761107236528757</v>
+        <v>5.5597925319379886</v>
       </c>
       <c r="AC12" s="1">
-        <v>-2.5109229776182103</v>
+        <v>-4.7982260789079865</v>
       </c>
       <c r="AD12" s="1">
-        <v>6.3856922604092752</v>
+        <v>3.6308539700841962</v>
       </c>
       <c r="AE12" s="1">
         <v>-2.4244985860035699</v>
@@ -1244,16 +1247,16 @@
         <v>5.9958782371607278</v>
       </c>
       <c r="AI12">
-        <v>4.4761107236528757</v>
+        <v>5.5597925319379886</v>
       </c>
       <c r="AJ12">
-        <v>5.9167212035742791</v>
+        <v>4.5832163444567335</v>
       </c>
       <c r="AK12">
-        <v>-0.72680727695228731</v>
+        <v>2.5752029212225906</v>
       </c>
       <c r="AL12">
-        <v>-4.1742250321537622</v>
+        <v>-3.8008848054569473</v>
       </c>
       <c r="AM12">
         <v>6.4987689843943119</v>
@@ -1331,13 +1334,13 @@
         <v>5.0420621306192057</v>
       </c>
       <c r="AB13" s="1">
-        <v>5.4488228950561926</v>
+        <v>7.1037817554960156</v>
       </c>
       <c r="AC13" s="1">
-        <v>7.352498798200406</v>
+        <v>2.141852422992446</v>
       </c>
       <c r="AD13" s="1">
-        <v>0.58332800921559014</v>
+        <v>-5.3886857445916938</v>
       </c>
       <c r="AE13" s="1">
         <v>8.5874721982909286</v>
@@ -1349,16 +1352,16 @@
         <v>5.0420621306192057</v>
       </c>
       <c r="AI13">
-        <v>5.4488228950561926</v>
+        <v>7.1037817554960156</v>
       </c>
       <c r="AJ13">
-        <v>-0.4610444456942111</v>
+        <v>-3.2395542851384769</v>
       </c>
       <c r="AK13">
-        <v>-6.7888012044549084</v>
+        <v>0.59296980107146746</v>
       </c>
       <c r="AL13">
-        <v>9.0467566080767092</v>
+        <v>9.8246536560289073</v>
       </c>
       <c r="AM13">
         <v>1.6359863117491964</v>
@@ -1890,16 +1893,16 @@
         <v>5.9958782371607278</v>
       </c>
       <c r="AB21">
-        <v>4.4761107236528757</v>
+        <v>5.5597925319379886</v>
       </c>
       <c r="AC21">
-        <v>5.9167212035742791</v>
+        <v>4.5832163444567335</v>
       </c>
       <c r="AD21">
-        <v>-0.72680727695228731</v>
+        <v>2.5752029212225906</v>
       </c>
       <c r="AE21">
-        <v>-4.1742250321537622</v>
+        <v>-3.8008848054569473</v>
       </c>
       <c r="AF21">
         <v>6.4987689843943119</v>
@@ -1909,19 +1912,19 @@
         <v>5.9958782371607278</v>
       </c>
       <c r="AI21">
-        <v>4.4761107236528757</v>
+        <v>5.5597925319379886</v>
       </c>
       <c r="AJ21">
-        <v>5.9167212035742791</v>
+        <v>4.5832163444567335</v>
       </c>
       <c r="AK21">
-        <v>2.994928739870188</v>
+        <v>1.1582372560522689</v>
       </c>
       <c r="AL21">
-        <v>3.8220751593618978</v>
+        <v>1.6029619965681543</v>
       </c>
       <c r="AM21">
-        <v>6.0504995718290608</v>
+        <v>7.7072299173310697</v>
       </c>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
@@ -1996,16 +1999,16 @@
         <v>5.0420621306192057</v>
       </c>
       <c r="AB22">
-        <v>5.4488228950561926</v>
+        <v>7.1037817554960156</v>
       </c>
       <c r="AC22">
-        <v>-0.4610444456942111</v>
+        <v>-3.2395542851384769</v>
       </c>
       <c r="AD22">
-        <v>-6.7888012044549084</v>
+        <v>0.59296980107146746</v>
       </c>
       <c r="AE22">
-        <v>9.0467566080767092</v>
+        <v>9.8246536560289073</v>
       </c>
       <c r="AF22">
         <v>1.6359863117491964</v>
@@ -2014,19 +2017,19 @@
         <v>5.0420621306192057</v>
       </c>
       <c r="AI22">
-        <v>5.4488228950561926</v>
+        <v>7.1037817554960156</v>
       </c>
       <c r="AJ22">
-        <v>-0.4610444456942111</v>
+        <v>-3.2395542851384769</v>
       </c>
       <c r="AK22">
-        <v>9.0983150427409818</v>
+        <v>4.9678951932620272</v>
       </c>
       <c r="AL22">
-        <v>-3.4329246414965668</v>
+        <v>-8.3476306210598317</v>
       </c>
       <c r="AM22">
-        <v>-6.003646385360951</v>
+        <v>-2.2779298104296286</v>
       </c>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
@@ -2530,42 +2533,42 @@
         <v>0</v>
       </c>
       <c r="AA30">
-        <f t="array" ref="AA30:AF35">MMULT(M30:R35,A30:F35)</f>
+        <f t="array" ref="AA30:AF35">MMULT(M30:R35,AH21:AM26)</f>
         <v>5.9958782371607278</v>
       </c>
       <c r="AB30">
-        <v>4.4761107236528757</v>
+        <v>5.5597925319379886</v>
       </c>
       <c r="AC30">
-        <v>-2.5109229776182103</v>
+        <v>4.5832163444567335</v>
       </c>
       <c r="AD30">
-        <v>6.3856922604092752</v>
+        <v>1.1582372560522689</v>
       </c>
       <c r="AE30">
-        <v>-2.4244985860035699</v>
+        <v>1.6029619965681543</v>
       </c>
       <c r="AF30">
-        <v>6.4987689843943119</v>
+        <v>7.7072299173310697</v>
       </c>
       <c r="AH30">
         <f t="array" ref="AH30:AM35">MMULT(AA30:AF35,TRANSPOSE(M30:R35))</f>
         <v>5.9958782371607278</v>
       </c>
       <c r="AI30">
-        <v>4.4761107236528757</v>
+        <v>5.5597925319379886</v>
       </c>
       <c r="AJ30">
-        <v>-2.5109229776182103</v>
+        <v>4.5832163444567335</v>
       </c>
       <c r="AK30">
-        <v>6.3856922604092752</v>
+        <v>1.1582372560522689</v>
       </c>
       <c r="AL30">
-        <v>3.6872945001438246</v>
+        <v>-1.3024696662894408E-2</v>
       </c>
       <c r="AM30">
-        <v>-5.8750362531024347</v>
+        <v>-7.8721477703560483</v>
       </c>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.25">
@@ -2622,37 +2625,37 @@
         <v>5.0420621306192057</v>
       </c>
       <c r="AB31">
-        <v>5.4488228950561926</v>
+        <v>7.1037817554960156</v>
       </c>
       <c r="AC31">
-        <v>7.352498798200406</v>
+        <v>-3.2395542851384769</v>
       </c>
       <c r="AD31">
-        <v>0.58332800921559014</v>
+        <v>4.9678951932620272</v>
       </c>
       <c r="AE31">
-        <v>8.5874721982909286</v>
+        <v>-8.3476306210598317</v>
       </c>
       <c r="AF31">
-        <v>1.6359863117491964</v>
+        <v>-2.2779298104296286</v>
       </c>
       <c r="AH31">
         <v>5.0420621306192057</v>
       </c>
       <c r="AI31">
-        <v>5.4488228950561926</v>
+        <v>7.1037817554960156</v>
       </c>
       <c r="AJ31">
-        <v>7.352498798200406</v>
+        <v>-3.2395542851384769</v>
       </c>
       <c r="AK31">
-        <v>0.58332800921559014</v>
+        <v>4.9678951932620272</v>
       </c>
       <c r="AL31">
-        <v>-8.0799628713870533</v>
+        <v>7.7153905111566097</v>
       </c>
       <c r="AM31">
-        <v>-3.3369641840536843</v>
+        <v>3.917224842570854</v>
       </c>
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.25">
@@ -2705,16 +2708,16 @@
         <v>4.5389254861480524</v>
       </c>
       <c r="AC32">
-        <v>1.5782006286162711</v>
+        <v>-0.73133264604650061</v>
       </c>
       <c r="AD32">
-        <v>-0.19342809951315143</v>
+        <v>1.1877221261656985</v>
       </c>
       <c r="AE32">
-        <v>0.50682434058115533</v>
+        <v>0.16406587775839898</v>
       </c>
       <c r="AF32">
-        <v>0.12025166748338001</v>
+        <v>-0.90940317196639586</v>
       </c>
       <c r="AH32">
         <v>2.8028508337126222E-16</v>
@@ -2723,16 +2726,16 @@
         <v>4.5389254861480524</v>
       </c>
       <c r="AJ32">
-        <v>1.5782006286162711</v>
+        <v>-0.73133264604650061</v>
       </c>
       <c r="AK32">
-        <v>-0.19342809951315143</v>
+        <v>1.1877221261656985</v>
       </c>
       <c r="AL32">
-        <v>-0.47208467178522451</v>
+        <v>-0.34438674053252677</v>
       </c>
       <c r="AM32">
-        <v>-0.22015321574642793</v>
+        <v>0.85751356512451649</v>
       </c>
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.25">
@@ -2788,13 +2791,13 @@
         <v>1.5741977039874566</v>
       </c>
       <c r="AD33">
-        <v>0.72792740626987551</v>
+        <v>-1.6128539368608326</v>
       </c>
       <c r="AE33">
-        <v>1.8186316379485974</v>
+        <v>-1.9037191376447509</v>
       </c>
       <c r="AF33">
-        <v>-2.9198251732723355</v>
+        <v>-2.4773441442679798</v>
       </c>
       <c r="AH33">
         <v>2.0953562842846303E-16</v>
@@ -2806,13 +2809,13 @@
         <v>1.5741977039874566</v>
       </c>
       <c r="AK33">
-        <v>0.72792740626987551</v>
+        <v>-1.6128539368608326</v>
       </c>
       <c r="AL33">
-        <v>-2.3709565112169955</v>
+        <v>1.3640397922360659</v>
       </c>
       <c r="AM33">
-        <v>2.4922610816164816</v>
+        <v>2.8108319069930729</v>
       </c>
     </row>
     <row r="34" spans="1:39" x14ac:dyDescent="0.25">
@@ -3145,6 +3148,175 @@
       </c>
       <c r="F44">
         <f t="shared" ref="F44" si="40">AM35</f>
+        <v>-4.5582918391073441</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>6</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f>AH30</f>
+        <v>5.9958782371607278</v>
+      </c>
+      <c r="B48">
+        <f t="shared" ref="B48:F48" si="41">AI30</f>
+        <v>5.5597925319379886</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="41"/>
+        <v>4.5832163444567335</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="41"/>
+        <v>1.1582372560522689</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="41"/>
+        <v>-1.3024696662894408E-2</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="41"/>
+        <v>-7.8721477703560483</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" ref="A49:A53" si="42">AH31</f>
+        <v>5.0420621306192057</v>
+      </c>
+      <c r="B49">
+        <f t="shared" ref="B49:B53" si="43">AI31</f>
+        <v>7.1037817554960156</v>
+      </c>
+      <c r="C49">
+        <f t="shared" ref="C49:C53" si="44">AJ31</f>
+        <v>-3.2395542851384769</v>
+      </c>
+      <c r="D49">
+        <f t="shared" ref="D49:D53" si="45">AK31</f>
+        <v>4.9678951932620272</v>
+      </c>
+      <c r="E49">
+        <f t="shared" ref="E49:E53" si="46">AL31</f>
+        <v>7.7153905111566097</v>
+      </c>
+      <c r="F49">
+        <f t="shared" ref="F49:F53" si="47">AM31</f>
+        <v>3.917224842570854</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="42"/>
+        <v>2.8028508337126222E-16</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="43"/>
+        <v>4.5389254861480524</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="44"/>
+        <v>-0.73133264604650061</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="45"/>
+        <v>1.1877221261656985</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="46"/>
+        <v>-0.34438674053252677</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="47"/>
+        <v>0.85751356512451649</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="42"/>
+        <v>2.0953562842846303E-16</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="43"/>
+        <v>-9.5619851380148667E-17</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="44"/>
+        <v>1.5741977039874566</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="45"/>
+        <v>-1.6128539368608326</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="46"/>
+        <v>1.3640397922360659</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="47"/>
+        <v>2.8108319069930729</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="42"/>
+        <v>-3.2925846313964868E-16</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="43"/>
+        <v>-1.5973850953025685E-16</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="44"/>
+        <v>8.6306586834697998E-17</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="45"/>
+        <v>5.6527251820119151</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="46"/>
+        <v>-1.3552645205599225</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="47"/>
+        <v>-7.5463524840688452</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="42"/>
+        <v>1.2507193846397565E-16</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="43"/>
+        <v>-1.2101346690101711E-16</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="44"/>
+        <v>1.3116049846314765E-16</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="46"/>
+        <v>-2.1777338051509885</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="47"/>
         <v>-4.5582918391073441</v>
       </c>
     </row>
@@ -3157,8 +3329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3554,30 +3726,30 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <f t="array" ref="P10:S13">MMULT(K10:N13,A10:D13)</f>
+        <f t="array" ref="P10:S13">MMULT(K10:N13,Z3:AC6)</f>
         <v>5.5103083596569142</v>
       </c>
       <c r="Q10">
-        <v>0.2228317660390795</v>
+        <v>2.9882369034928025E-2</v>
       </c>
       <c r="R10">
-        <v>6.3833407742313035</v>
+        <v>5.8743714896548838</v>
       </c>
       <c r="S10">
-        <v>1.0121404990342597</v>
+        <v>2.7040688732456566</v>
       </c>
       <c r="U10">
         <f t="array" ref="U10:X13">MMULT(P10:S13,TRANSPOSE(K10:N13))</f>
         <v>5.5103083596569142</v>
       </c>
       <c r="V10">
-        <v>0.2228317660390795</v>
+        <v>2.9882369034928025E-2</v>
       </c>
       <c r="W10">
-        <v>5.832760124171732</v>
+        <v>6.3723500865403944</v>
       </c>
       <c r="X10">
-        <v>-2.7839499211769927</v>
+        <v>-1.1015367648402865</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
@@ -3620,25 +3792,25 @@
         <v>5.9498502790165215</v>
       </c>
       <c r="Q11">
-        <v>6.376892811209844</v>
+        <v>5.5465726781654077</v>
       </c>
       <c r="R11">
-        <v>4.0880483017860483</v>
+        <v>6.4082239141550144</v>
       </c>
       <c r="S11">
-        <v>4.3766866671310076</v>
+        <v>-2.1685213435700179</v>
       </c>
       <c r="U11">
         <v>5.9498502790165215</v>
       </c>
       <c r="V11">
-        <v>6.376892811209844</v>
+        <v>5.5465726781654077</v>
       </c>
       <c r="W11">
-        <v>5.8486070699875317</v>
+        <v>4.0505831425464365</v>
       </c>
       <c r="X11">
-        <v>1.2889222012480013</v>
+        <v>-5.4185417555635365</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
@@ -3847,8 +4019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4788,27 +4960,27 @@
         <v>0</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B14:B19" si="8">AM6</f>
+        <f t="shared" ref="B16:B19" si="8">AM6</f>
         <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C14:C19" si="9">AN6</f>
+        <f t="shared" ref="C16:C19" si="9">AN6</f>
         <v>3.1696987831541712</v>
       </c>
       <c r="D16">
-        <f t="shared" ref="D14:D19" si="10">AO6</f>
+        <f t="shared" ref="D16:D19" si="10">AO6</f>
         <v>2.802908177741934</v>
       </c>
       <c r="E16">
-        <f t="shared" ref="E14:E19" si="11">AP6</f>
+        <f t="shared" ref="E16:E19" si="11">AP6</f>
         <v>-4.8233400275995804</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F14:F19" si="12">AQ6</f>
+        <f t="shared" ref="F16:F19" si="12">AQ6</f>
         <v>1.8476786301004875</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" ref="G14:G19" si="13">AR6</f>
+        <f t="shared" ref="G16:G19" si="13">AR6</f>
         <v>7.0278408432760431</v>
       </c>
     </row>
@@ -7763,8 +7935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7772,799 +7944,799 @@
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND()*10-3</f>
-        <v>5.5501888492991824</v>
+        <v>6.5338650847697242</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:J16" ca="1" si="0">RAND()*10-3</f>
-        <v>-1.2488782277171291</v>
+        <v>1.5724255605768915</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6140556765653535</v>
+        <v>-1.4684815470943287</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2891621545191905</v>
+        <v>4.4244795590251931</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>5.408184851142197</v>
+        <v>1.0855116824247517</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5852597785234046</v>
+        <v>1.8126212716979584</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2696330704222962</v>
+        <v>5.34817329015981</v>
       </c>
       <c r="H1">
         <f ca="1">RAND()*10-3</f>
-        <v>2.0792433840949371</v>
+        <v>2.8398492136494182</v>
       </c>
       <c r="I1">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.0651585215506527</v>
+        <v>4.9168857882797496</v>
       </c>
       <c r="J1">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.7791500128439646</v>
+        <v>-0.35191850996377649</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:J19" ca="1" si="1">RAND()*10-3</f>
-        <v>3.4043263337069991</v>
+        <v>-2.3039740716229238</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2215255826061</v>
+        <v>5.5798950193127386</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>4.341547399736621</v>
+        <v>-2.7019813357663001</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3101520033325325</v>
+        <v>2.5520897648757632</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1837006492656927</v>
+        <v>-1.3282841827702447</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8723980732013503</v>
+        <v>6.3070565538504653</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>5.335512989148782</v>
+        <v>1.7603886051780648E-2</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6524972798736268</v>
+        <v>5.9421979131859111</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.875186299511336</v>
+        <v>5.9455089487469905</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2705781036226806</v>
+        <v>6.9744537482934703</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.6789369367025131E-3</v>
+        <v>3.2118066179993505</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.12185488020789625</v>
+        <v>-2.1618293409497298</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.1026356663233901</v>
+        <v>4.2497632851105944</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.4266271397264632</v>
+        <v>-1.7328349611070244</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6753667858877463</v>
+        <v>4.1839456539863509</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.2538364169691079E-2</v>
+        <v>6.4380222258444437</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.9301667786438488</v>
+        <v>6.2536166711262737</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1711035877710678</v>
+        <v>2.2650917923157294</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6254552847005677</v>
+        <v>2.44109797585421</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19556069047563396</v>
+        <v>0.51021251404740475</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5171231440063178</v>
+        <v>2.1105485932787831</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2095137353725542</v>
+        <v>3.8111527487297776</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6731502743499629</v>
+        <v>0.76168731417017232</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.5202368054628586</v>
+        <v>1.2540567773150322</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.1694753346790927</v>
+        <v>3.0052281629078834</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1281971111642832</v>
+        <v>1.8603250691068034</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0164243262045636</v>
+        <v>6.3311793152299565</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2783632037429564</v>
+        <v>5.1127046603834749</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7465834812617853</v>
+        <v>-2.361616249676902</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.57582917874337269</v>
+        <v>-0.41830868956306588</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.7886950201761027</v>
+        <v>-2.9679278226354171</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7804498958326438</v>
+        <v>5.6457058455580498</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>3.280175220520503</v>
+        <v>-1.0307060687904974</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0939388412261479</v>
+        <v>-0.85699678446747596</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.1314913698421665</v>
+        <v>-1.8542775103143023</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0460749116592654</v>
+        <v>4.8184469244488799</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.4741194233961625</v>
+        <v>-1.5939384988264411</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3870267973078683</v>
+        <v>-1.2394719974328656</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3533391446178982</v>
+        <v>0.72965302963306211</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6922280358111772</v>
+        <v>6.3081116943230509</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.4831615539751071</v>
+        <v>6.2887179401958182</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.3534163887166679</v>
+        <v>2.7359741387455578</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8280315691605589</v>
+        <v>1.6712457085442827</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0980868357781493</v>
+        <v>-9.6120783101827811E-2</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.4140096537537101</v>
+        <v>3.4176852908325888</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7382882153273442</v>
+        <v>4.2305103269019302</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.6094169635987816</v>
+        <v>5.8471430882924089</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5845016207671616</v>
+        <v>6.9923458361434729</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2830917136676856</v>
+        <v>-1.5337141099167046</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8954462653932147</v>
+        <v>6.747051520759479</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5402058218877199</v>
+        <v>3.2594992982963413</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.9458522263248408</v>
+        <v>0.33376504797959239</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.2836352137938318</v>
+        <v>2.5458235602538721</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7995868381744458</v>
+        <v>3.9997651607531539</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4792895008005198</v>
+        <v>2.8481442859855388</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8801357341733196</v>
+        <v>1.5590639364840619</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3398536087195474</v>
+        <v>1.4823001731443419</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8876751398610825</v>
+        <v>6.1908113173435328</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.8248174167048532</v>
+        <v>5.2565993180744375</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.20549958395182166</v>
+        <v>2.9278915847485028</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.2101473782561296</v>
+        <v>4.6618489403588663</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.5329883794556389</v>
+        <v>5.1405156838249813</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>2.659353978351966</v>
+        <v>1.3107485478571039</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5466239580182748</v>
+        <v>1.9042559309238518</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0884575951869824</v>
+        <v>3.0438473727160069</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7388867130293146</v>
+        <v>0.41582202103408594</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7250062617320694</v>
+        <v>2.8993409052863468</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7533804734139586</v>
+        <v>5.0435860123063634</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2835261398601503</v>
+        <v>5.7691931565501164</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.530748524121986</v>
+        <v>0.24272382196593512</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.19382285016819445</v>
+        <v>4.8467204363201857</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84789950125164282</v>
+        <v>-1.401093671242299</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3745808243857747</v>
+        <v>-2.1392157374054115</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.69443630425403757</v>
+        <v>6.2015675245280573</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1816755609739058</v>
+        <v>6.6008899471546787</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0513662701913251</v>
+        <v>2.047670973276289</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8828096307043971</v>
+        <v>3.6971389251641664</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.77857439899409808</v>
+        <v>1.124652942093185</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1807064068772277</v>
+        <v>2.3090911091662267</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3166231010213281</v>
+        <v>1.3637692796238161</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1289961027429332</v>
+        <v>5.2008491933605008</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.2174211230078265</v>
+        <v>-0.31153958351361988</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.9967624249168765</v>
+        <v>-2.9326909971914947</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0922823850142169</v>
+        <v>1.6517982862677556</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0633727247417477</v>
+        <v>5.787098301807438</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.51661650773284817</v>
+        <v>6.4356973795691204</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>4.6627948816309832</v>
+        <v>-0.46752771722853836</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.89688322043913349</v>
+        <v>-2.1955903372909189</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2534254596987822E-2</v>
+        <v>3.8446027373995602</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6864484357271898</v>
+        <v>0.28599729408322183</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16114428769340483</v>
+        <v>2.8687066186652537</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2376638207189856</v>
+        <v>-1.233042514346478</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5793095986967085</v>
+        <v>4.4905145061080516</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.6582155439626307</v>
+        <v>3.0262710889672633</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5209918675228593</v>
+        <v>3.9406634036005972</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2107351182111774</v>
+        <v>5.3430292237151171</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0389292420541043</v>
+        <v>4.8102749798657998</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6631274979263093</v>
+        <v>-2.3266081200464432</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0251535692577978</v>
+        <v>4.9876909205319624</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5101080975308783</v>
+        <v>6.9708765926669543</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.44891332451523835</v>
+        <v>3.1596460839860478</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8161731328168411</v>
+        <v>1.5885302457819188</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7811912367379801</v>
+        <v>-2.7393574656273496</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3573981520143414</v>
+        <v>5.1044334480707896</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1378013411022696</v>
+        <v>4.1634084172039998</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6693591580382829</v>
+        <v>0.25792601064294418</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29423474469097233</v>
+        <v>0.28111008706534202</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8011434074981256</v>
+        <v>2.7587356685737925</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.65972546390006137</v>
+        <v>5.4119771573353095</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.601819744279414</v>
+        <v>-0.96817959910065099</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>6.2102700911948041</v>
+        <v>5.5555857668224675</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2614615340505759</v>
+        <v>-2.0181024646597718</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.34910497097130611</v>
+        <v>5.6864945614180336</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.68462836200539234</v>
+        <v>4.34290115053318</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.95847761282331678</v>
+        <v>5.3878937830671578</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5303094949223119</v>
+        <v>6.0441557796872658</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1720475189065027</v>
+        <v>6.7667172703636567</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4748650357641768</v>
+        <v>-1.0645156331442736</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6892051623777897</v>
+        <v>-1.1669266286678621</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1710247565330576</v>
+        <v>0.75091847844858828</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>5.086012727282009</v>
+        <v>5.3590772704280898</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>4.6136503881559259</v>
+        <v>4.7904364590145221</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1248316892601622</v>
+        <v>-0.23740052303746495</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7628129688750125</v>
+        <v>5.1235878070951681</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6530341686989418</v>
+        <v>5.5885208563392226</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>5.4715116097271164</v>
+        <v>-2.4852863473141715</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1725265101749063</v>
+        <v>2.23093229733621</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0844979487273223</v>
+        <v>5.1247002971110529</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.5157892726113804</v>
+        <v>1.8598321452089017</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8562463016513409</v>
+        <v>-2.3275880120470234</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69748367239864173</v>
+        <v>6.4409099865772443</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3303464414672401</v>
+        <v>4.8310325290092972</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.3987126280341506</v>
+        <v>-5.7030691728865435E-4</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.5305712198066441</v>
+        <v>6.9537891415861317</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>2.004946340372209</v>
+        <v>-1.5453519145889589</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8860551721773344</v>
+        <v>3.6089670061859964</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.9285797980784187</v>
+        <v>0.59740640386725818</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7059662901968453</v>
+        <v>2.85431599533133</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2519267512229151</v>
+        <v>0.34167523380348497</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.3791996504916764E-2</v>
+        <v>-2.1216033244504446</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.2743405248572</v>
+        <v>3.0723039659851663</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21511783197106915</v>
+        <v>-2.6291089723033352</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.738946868997618</v>
+        <v>4.3485443937382868</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5716471618419909</v>
+        <v>5.0663511460145028</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8172873150887332</v>
+        <v>1.9370292595195684</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1705810733972557</v>
+        <v>2.3634381375583997</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7244758192321381</v>
+        <v>-2.5851720603501178</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5523751274083892</v>
+        <v>-0.88119851900638135</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0534945587935987</v>
+        <v>6.4315307325970608</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.8626685879395595</v>
+        <v>6.837984910085158</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.6521348627245098</v>
+        <v>3.634366975405765</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8025663263035892</v>
+        <v>8.0571672091527713E-2</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.0016937183212633</v>
+        <v>0.49213136335741803</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>5.4680209193266425</v>
+        <v>-0.26063049627387525</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1179319991182801</v>
+        <v>-1.7118906519350647</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>6.3893758326194483</v>
+        <v>-1.932016741343044</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8027465487162342</v>
+        <v>-1.9812558689461164</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7581915822849936</v>
+        <v>-2.4313682567149137</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.7711947614358841</v>
+        <v>4.8693087462373734</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.38867132625859124</v>
+        <v>-2.4694845624358015</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.022622834456536</v>
+        <v>2.2210952466808447</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4412570702023553</v>
+        <v>-1.6867330721825575</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>4.4330234817812126</v>
+        <v>5.8713122705984784</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.49075619622076427</v>
+        <v>-0.2154006166343998</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8873852376424605</v>
+        <v>2.2246554637569256</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9574075853216186</v>
+        <v>0.12656769523761868</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>4.4114696926396162</v>
+        <v>-0.16470888122400007</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5762309941906105</v>
+        <v>0.72117117760458083</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.9577050225381649</v>
+        <v>3.150665402039758</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.88084619601303071</v>
+        <v>0.85331782510886267</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0314536944999073</v>
+        <v>-1.567220543354902</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0467668902463121</v>
+        <v>2.0029581792862601</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>5.6514578498709476</v>
+        <v>4.7579398330084466</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2757141925514635</v>
+        <v>1.367454760296595</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.28280179815331241</v>
+        <v>-0.85964544556675193</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>3.6020718269704073</v>
+        <v>5.4169370529491978</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>6.499120171323403</v>
+        <v>1.8783284480250657</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2476492501263099</v>
+        <v>-0.32608686019933586</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.9890532620234875</v>
+        <v>1.7955221563897279</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.8465324818739797</v>
+        <v>-1.5564007385151419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bulge chaser batch rotate
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/BulgeChaserTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/BulgeChaserTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-240" yWindow="1605" windowWidth="19440" windowHeight="11040" activeTab="4"/>
+    <workbookView xWindow="-240" yWindow="1605" windowWidth="19440" windowHeight="11040" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="By Diag 6x6" sheetId="1" r:id="rId1"/>
@@ -5083,8 +5083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM53"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:F53"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5093,8 +5093,9 @@
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="32" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="34" max="35" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="36" max="39" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -5830,17 +5831,17 @@
         <v>0</v>
       </c>
       <c r="AA12" s="1">
-        <f t="array" ref="AA12:AF17">MMULT(T12:Y17,MMULT(M12:R17,A12:F17))</f>
+        <f t="array" ref="AA12:AF17">MMULT(T12:Y17,MMULT(M12:R17,AH3:AM8))</f>
         <v>-2.4894028533397057</v>
       </c>
       <c r="AB12" s="1">
-        <v>-1.2208340311620398</v>
+        <v>5.2412859060773114</v>
       </c>
       <c r="AC12" s="1">
-        <v>5.4870796290101254</v>
+        <v>1.5164626433619954</v>
       </c>
       <c r="AD12" s="1">
-        <v>1.5227302569475185</v>
+        <v>2.0362831640534669</v>
       </c>
       <c r="AE12" s="1">
         <v>-1.9860942179327741</v>
@@ -5853,16 +5854,16 @@
         <v>-2.4894028533397057</v>
       </c>
       <c r="AI12">
-        <v>-1.2208340311620398</v>
+        <v>5.2412859060773114</v>
       </c>
       <c r="AJ12">
-        <v>-2.6108953358522795</v>
+        <v>0.4736861443281063</v>
       </c>
       <c r="AK12">
-        <v>-5.05026711204746</v>
+        <v>-2.4980246279095346</v>
       </c>
       <c r="AL12">
-        <v>-2.0122992260655406</v>
+        <v>-1.9814572189313224</v>
       </c>
       <c r="AM12">
         <v>3.1912023760579356</v>
@@ -5940,13 +5941,13 @@
         <v>6.2548854525046629</v>
       </c>
       <c r="AB13" s="1">
-        <v>-1.643246018611362</v>
+        <v>3.6095045673011934</v>
       </c>
       <c r="AC13" s="1">
-        <v>3.9828265381920192</v>
+        <v>1.8567166172206244</v>
       </c>
       <c r="AD13" s="1">
-        <v>2.707090150224551</v>
+        <v>3.0684820309755971</v>
       </c>
       <c r="AE13" s="1">
         <v>-0.74689736061406387</v>
@@ -5958,16 +5959,16 @@
         <v>6.2548854525046629</v>
       </c>
       <c r="AI13">
-        <v>-1.643246018611362</v>
+        <v>3.6095045673011934</v>
       </c>
       <c r="AJ13">
-        <v>-0.731159215011423</v>
+        <v>0.9836748790001647</v>
       </c>
       <c r="AK13">
-        <v>-4.7587414390454628</v>
+        <v>-3.4510727024994639</v>
       </c>
       <c r="AL13">
-        <v>-0.75424538492261073</v>
+        <v>-0.73709916080717164</v>
       </c>
       <c r="AM13">
         <v>2.7668549840000694</v>
@@ -6499,16 +6500,16 @@
         <v>-2.4894028533397057</v>
       </c>
       <c r="AB21">
-        <v>-1.2208340311620398</v>
+        <v>5.2412859060773114</v>
       </c>
       <c r="AC21">
-        <v>-2.6108953358522795</v>
+        <v>0.4736861443281063</v>
       </c>
       <c r="AD21">
-        <v>-5.05026711204746</v>
+        <v>-2.4980246279095346</v>
       </c>
       <c r="AE21">
-        <v>-2.0122992260655406</v>
+        <v>-1.9814572189313224</v>
       </c>
       <c r="AF21">
         <v>3.1912023760579356</v>
@@ -6518,19 +6519,19 @@
         <v>-2.4894028533397057</v>
       </c>
       <c r="AI21">
-        <v>-1.2208340311620398</v>
+        <v>5.2412859060773114</v>
       </c>
       <c r="AJ21">
-        <v>-2.6108953358522795</v>
+        <v>0.4736861443281063</v>
       </c>
       <c r="AK21">
-        <v>-5.3475893166021393</v>
+        <v>-2.8375477349213827</v>
       </c>
       <c r="AL21">
-        <v>-0.99784093618018366</v>
+        <v>-1.4610648741962005</v>
       </c>
       <c r="AM21">
-        <v>3.1852661820098636</v>
+        <v>3.1880534252876012</v>
       </c>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
@@ -6605,16 +6606,16 @@
         <v>6.2548854525046629</v>
       </c>
       <c r="AB22">
-        <v>-1.643246018611362</v>
+        <v>3.6095045673011934</v>
       </c>
       <c r="AC22">
-        <v>-0.731159215011423</v>
+        <v>0.9836748790001647</v>
       </c>
       <c r="AD22">
-        <v>-4.7587414390454628</v>
+        <v>-3.4510727024994639</v>
       </c>
       <c r="AE22">
-        <v>-0.75424538492261073</v>
+        <v>-0.73709916080717164</v>
       </c>
       <c r="AF22">
         <v>2.7668549840000694</v>
@@ -6623,19 +6624,19 @@
         <v>6.2548854525046629</v>
       </c>
       <c r="AI22">
-        <v>-1.643246018611362</v>
+        <v>3.6095045673011934</v>
       </c>
       <c r="AJ22">
-        <v>-0.731159215011423</v>
+        <v>0.9836748790001647</v>
       </c>
       <c r="AK22">
-        <v>-4.817845490719221</v>
+        <v>-3.5315389731453597</v>
       </c>
       <c r="AL22">
-        <v>0.18010508920946466</v>
+        <v>-5.591402054414607E-2</v>
       </c>
       <c r="AM22">
-        <v>2.7615067755210911</v>
+        <v>2.7629351379914122</v>
       </c>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
@@ -7139,42 +7140,42 @@
         <v>0</v>
       </c>
       <c r="AA30">
-        <f t="array" ref="AA30:AF35">MMULT(M30:R35,A30:F35)</f>
+        <f t="array" ref="AA30:AF35">MMULT(M30:R35,AH21:AM26)</f>
         <v>-2.4894028533397057</v>
       </c>
       <c r="AB30">
-        <v>-1.2208340311620398</v>
+        <v>5.2412859060773114</v>
       </c>
       <c r="AC30">
-        <v>5.4870796290101254</v>
+        <v>0.4736861443281063</v>
       </c>
       <c r="AD30">
-        <v>1.5227302569475185</v>
+        <v>-2.8375477349213827</v>
       </c>
       <c r="AE30">
-        <v>-1.9860942179327741</v>
+        <v>-1.4610648741962005</v>
       </c>
       <c r="AF30">
-        <v>3.1912023760579356</v>
+        <v>3.1880534252876012</v>
       </c>
       <c r="AH30">
         <f t="array" ref="AH30:AM35">MMULT(AA30:AF35,TRANSPOSE(M30:R35))</f>
         <v>-2.4894028533397057</v>
       </c>
       <c r="AI30">
-        <v>-1.2208340311620398</v>
+        <v>5.2412859060773114</v>
       </c>
       <c r="AJ30">
-        <v>5.4870796290101254</v>
+        <v>0.4736861443281063</v>
       </c>
       <c r="AK30">
-        <v>1.5227302569475185</v>
+        <v>-2.8375477349213827</v>
       </c>
       <c r="AL30">
-        <v>2.1400608638413559</v>
+        <v>1.6155077772351196</v>
       </c>
       <c r="AM30">
-        <v>-3.0900618677493177</v>
+        <v>-3.1126403311000792</v>
       </c>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.25">
@@ -7231,37 +7232,37 @@
         <v>6.2548854525046629</v>
       </c>
       <c r="AB31">
-        <v>-1.643246018611362</v>
+        <v>3.6095045673011934</v>
       </c>
       <c r="AC31">
-        <v>3.9828265381920192</v>
+        <v>0.9836748790001647</v>
       </c>
       <c r="AD31">
-        <v>2.707090150224551</v>
+        <v>-3.5315389731453597</v>
       </c>
       <c r="AE31">
-        <v>-0.74689736061406387</v>
+        <v>-5.591402054414607E-2</v>
       </c>
       <c r="AF31">
-        <v>2.7668549840000694</v>
+        <v>2.7629351379914122</v>
       </c>
       <c r="AH31">
         <v>6.2548854525046629</v>
       </c>
       <c r="AI31">
-        <v>-1.643246018611362</v>
+        <v>3.6095045673011934</v>
       </c>
       <c r="AJ31">
-        <v>3.9828265381920192</v>
+        <v>0.9836748790001647</v>
       </c>
       <c r="AK31">
-        <v>2.707090150224551</v>
+        <v>-3.5315389731453597</v>
       </c>
       <c r="AL31">
-        <v>0.88156147683784747</v>
+        <v>0.19121592815199892</v>
       </c>
       <c r="AM31">
-        <v>-2.7269381240383423</v>
+        <v>-2.7568774770130799</v>
       </c>
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.25">
@@ -7314,16 +7315,16 @@
         <v>9.116971882329846</v>
       </c>
       <c r="AC32">
-        <v>-2.5868707679759351</v>
+        <v>2.5893866774993231</v>
       </c>
       <c r="AD32">
-        <v>1.1216293372563073</v>
+        <v>1.0188744917087902</v>
       </c>
       <c r="AE32">
-        <v>-0.44411079277801158</v>
+        <v>-0.62801906340275659</v>
       </c>
       <c r="AF32">
-        <v>4.2984630141770257</v>
+        <v>4.2995970603591545</v>
       </c>
       <c r="AH32">
         <v>0</v>
@@ -7332,16 +7333,16 @@
         <v>9.116971882329846</v>
       </c>
       <c r="AJ32">
-        <v>-2.5868707679759351</v>
+        <v>2.5893866774993231</v>
       </c>
       <c r="AK32">
-        <v>1.1216293372563073</v>
+        <v>1.0188744917087902</v>
       </c>
       <c r="AL32">
-        <v>0.65417915271880289</v>
+        <v>0.8379221191922519</v>
       </c>
       <c r="AM32">
-        <v>-4.2715416791432421</v>
+        <v>-4.2636638408315832</v>
       </c>
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.25">
@@ -7397,13 +7398,13 @@
         <v>3.7201259357316556</v>
       </c>
       <c r="AD33">
-        <v>4.1596529774853686</v>
+        <v>4.509955193792214</v>
       </c>
       <c r="AE33">
-        <v>2.2057695494085867</v>
+        <v>1.3598633095255321</v>
       </c>
       <c r="AF33">
-        <v>-2.0788917112384273</v>
+        <v>-2.0738849714122982</v>
       </c>
       <c r="AH33">
         <v>0</v>
@@ -7415,13 +7416,13 @@
         <v>3.7201259357316556</v>
       </c>
       <c r="AK33">
-        <v>4.1596529774853686</v>
+        <v>4.509955193792214</v>
       </c>
       <c r="AL33">
-        <v>-2.3049750952107559</v>
+        <v>-1.4598394508253105</v>
       </c>
       <c r="AM33">
-        <v>1.9683241253950434</v>
+        <v>2.0047682841310057</v>
       </c>
     </row>
     <row r="34" spans="1:39" x14ac:dyDescent="0.25">
@@ -7777,23 +7778,23 @@
       </c>
       <c r="B48">
         <f t="shared" ref="B48:F48" si="13">AI30</f>
-        <v>-1.2208340311620398</v>
+        <v>5.2412859060773114</v>
       </c>
       <c r="C48">
         <f t="shared" si="13"/>
-        <v>5.4870796290101254</v>
+        <v>0.4736861443281063</v>
       </c>
       <c r="D48">
         <f t="shared" si="13"/>
-        <v>1.5227302569475185</v>
+        <v>-2.8375477349213827</v>
       </c>
       <c r="E48">
         <f t="shared" si="13"/>
-        <v>2.1400608638413559</v>
+        <v>1.6155077772351196</v>
       </c>
       <c r="F48">
         <f t="shared" si="13"/>
-        <v>-3.0900618677493177</v>
+        <v>-3.1126403311000792</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -7803,23 +7804,23 @@
       </c>
       <c r="B49">
         <f t="shared" ref="B49:B53" si="15">AI31</f>
-        <v>-1.643246018611362</v>
+        <v>3.6095045673011934</v>
       </c>
       <c r="C49">
         <f t="shared" ref="C49:C53" si="16">AJ31</f>
-        <v>3.9828265381920192</v>
+        <v>0.9836748790001647</v>
       </c>
       <c r="D49">
         <f t="shared" ref="D49:D53" si="17">AK31</f>
-        <v>2.707090150224551</v>
+        <v>-3.5315389731453597</v>
       </c>
       <c r="E49">
         <f t="shared" ref="E49:E53" si="18">AL31</f>
-        <v>0.88156147683784747</v>
+        <v>0.19121592815199892</v>
       </c>
       <c r="F49">
         <f t="shared" ref="F49:F53" si="19">AM31</f>
-        <v>-2.7269381240383423</v>
+        <v>-2.7568774770130799</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -7833,19 +7834,19 @@
       </c>
       <c r="C50">
         <f t="shared" si="16"/>
-        <v>-2.5868707679759351</v>
+        <v>2.5893866774993231</v>
       </c>
       <c r="D50">
         <f t="shared" si="17"/>
-        <v>1.1216293372563073</v>
+        <v>1.0188744917087902</v>
       </c>
       <c r="E50">
         <f t="shared" si="18"/>
-        <v>0.65417915271880289</v>
+        <v>0.8379221191922519</v>
       </c>
       <c r="F50">
         <f t="shared" si="19"/>
-        <v>-4.2715416791432421</v>
+        <v>-4.2636638408315832</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -7863,15 +7864,15 @@
       </c>
       <c r="D51">
         <f t="shared" si="17"/>
-        <v>4.1596529774853686</v>
+        <v>4.509955193792214</v>
       </c>
       <c r="E51">
         <f t="shared" si="18"/>
-        <v>-2.3049750952107559</v>
+        <v>-1.4598394508253105</v>
       </c>
       <c r="F51">
         <f t="shared" si="19"/>
-        <v>1.9683241253950434</v>
+        <v>2.0047682841310057</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -7935,7 +7936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5:H8"/>
     </sheetView>
   </sheetViews>
@@ -7944,799 +7945,799 @@
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND()*10-3</f>
-        <v>6.5338650847697242</v>
+        <v>-0.38359501537838581</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:J16" ca="1" si="0">RAND()*10-3</f>
-        <v>1.5724255605768915</v>
+        <v>0.53848117489840464</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.4684815470943287</v>
+        <v>-0.48831023151230069</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4244795590251931</v>
+        <v>1.3156616284243032</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0855116824247517</v>
+        <v>-1.6517580557681695</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8126212716979584</v>
+        <v>-1.0163508720970689</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>5.34817329015981</v>
+        <v>-1.7106287160216156</v>
       </c>
       <c r="H1">
         <f ca="1">RAND()*10-3</f>
-        <v>2.8398492136494182</v>
+        <v>3.5142311047359023</v>
       </c>
       <c r="I1">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9168857882797496</v>
+        <v>-1.6079891175597489</v>
       </c>
       <c r="J1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.35191850996377649</v>
+        <v>-2.456344037716268</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:J19" ca="1" si="1">RAND()*10-3</f>
-        <v>-2.3039740716229238</v>
+        <v>5.2951193027848031</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5798950193127386</v>
+        <v>1.5200264381873776</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.7019813357663001</v>
+        <v>2.1332102958984471</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5520897648757632</v>
+        <v>0.2257935668461748</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.3282841827702447</v>
+        <v>5.1291768640166957</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3070565538504653</v>
+        <v>0.61551012421407636</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7603886051780648E-2</v>
+        <v>5.5405708457929137</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>5.9421979131859111</v>
+        <v>5.9658745302591676</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>5.9455089487469905</v>
+        <v>1.9818216291691284</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9744537482934703</v>
+        <v>6.2046070007102934</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2118066179993505</v>
+        <v>-1.6458359926136874</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1618293409497298</v>
+        <v>-2.36785392506988</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2497632851105944</v>
+        <v>6.5744061433321797</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7328349611070244</v>
+        <v>5.933387702138436</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1839456539863509</v>
+        <v>2.7304806693276644</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4380222258444437</v>
+        <v>4.1195028362955526</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2536166711262737</v>
+        <v>6.6387680374151614</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2650917923157294</v>
+        <v>-0.32648985616896375</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.44109797585421</v>
+        <v>-0.35937780381745954</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.51021251404740475</v>
+        <v>3.2525009652220938</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1105485932787831</v>
+        <v>-1.002649552835851</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8111527487297776</v>
+        <v>4.0197997195020081</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.76168731417017232</v>
+        <v>2.5718695463503742</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2540567773150322</v>
+        <v>1.7539967407592769</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0052281629078834</v>
+        <v>-0.32751882526938569</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8603250691068034</v>
+        <v>4.9529950323954557</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3311793152299565</v>
+        <v>-1.2539824289867203</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1127046603834749</v>
+        <v>2.4057691896713749</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.361616249676902</v>
+        <v>5.6123699793623629</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.41830868956306588</v>
+        <v>4.1180611212434659</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.9679278226354171</v>
+        <v>5.7813273690552158</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6457058455580498</v>
+        <v>-0.43402327160258647</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.0307060687904974</v>
+        <v>4.2486709499763737</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.85699678446747596</v>
+        <v>-1.2301564807280536</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.8542775103143023</v>
+        <v>5.2906208229676039</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8184469244488799</v>
+        <v>6.3678814229041958</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.5939384988264411</v>
+        <v>2.258715959621191</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.2394719974328656</v>
+        <v>-0.86226982835533494</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72965302963306211</v>
+        <v>1.350088078025351</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3081116943230509</v>
+        <v>6.1703122999818838</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>6.2887179401958182</v>
+        <v>-0.46367092718527392</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7359741387455578</v>
+        <v>6.5312969258749813</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6712457085442827</v>
+        <v>0.3674859775959467</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.6120783101827811E-2</v>
+        <v>-0.70172213117501592</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4176852908325888</v>
+        <v>-1.4023991672928233</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2305103269019302</v>
+        <v>-2.4866507207201431</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8471430882924089</v>
+        <v>-0.16343010615476317</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9923458361434729</v>
+        <v>-2.9181924652303834</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.5337141099167046</v>
+        <v>-2.8408882171742533E-2</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.747051520759479</v>
+        <v>5.2682011677714478</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2594992982963413</v>
+        <v>-2.9472974562490224</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33376504797959239</v>
+        <v>0.34904158249242112</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5458235602538721</v>
+        <v>3.266817508921295</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9997651607531539</v>
+        <v>0.25954365607038277</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8481442859855388</v>
+        <v>-0.76128427756078132</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5590639364840619</v>
+        <v>4.1000811026028074</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4823001731443419</v>
+        <v>1.9105376564883851</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1908113173435328</v>
+        <v>5.1962195710270098</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2565993180744375</v>
+        <v>2.0854499683790513</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9278915847485028</v>
+        <v>5.473091568882511</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.6618489403588663</v>
+        <v>6.7633867664841496</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1405156838249813</v>
+        <v>-1.1728153010148041</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3107485478571039</v>
+        <v>6.0761156514756909</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9042559309238518</v>
+        <v>1.8162283992485637</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0438473727160069</v>
+        <v>-2.3617205511543009</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41582202103408594</v>
+        <v>6.7371053804915668</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8993409052863468</v>
+        <v>-2.0192470549952475</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0435860123063634</v>
+        <v>-0.71356686802729818</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7691931565501164</v>
+        <v>1.450258747157303</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.24272382196593512</v>
+        <v>5.7808952575906005</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8467204363201857</v>
+        <v>-0.42856109510529627</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.401093671242299</v>
+        <v>2.7830933567128788</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1392157374054115</v>
+        <v>-0.25714011174117068</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2015675245280573</v>
+        <v>-1.2632137095731484</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6008899471546787</v>
+        <v>-0.40107288557074838</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.047670973276289</v>
+        <v>-2.5134982299152249</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6971389251641664</v>
+        <v>0.93649941854388397</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.124652942093185</v>
+        <v>6.3670728572225492</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3090911091662267</v>
+        <v>0.81114395694911767</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3637692796238161</v>
+        <v>-1.6370034785709182</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>5.2008491933605008</v>
+        <v>-0.83465845457814591</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.31153958351361988</v>
+        <v>1.2897243910333067</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.9326909971914947</v>
+        <v>2.3409671781995014</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6517982862677556</v>
+        <v>-1.9585947972077229</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>5.787098301807438</v>
+        <v>3.0038038361103503</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4356973795691204</v>
+        <v>-2.2205376122308822</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.46752771722853836</v>
+        <v>2.3022047812868136</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1955903372909189</v>
+        <v>0.95524240906279356</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8446027373995602</v>
+        <v>5.0583706158935602</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28599729408322183</v>
+        <v>-6.2717016201085496E-2</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8687066186652537</v>
+        <v>4.7612978816469411</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.233042514346478</v>
+        <v>0.69685395251094562</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4905145061080516</v>
+        <v>2.5084947949306944</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0262710889672633</v>
+        <v>2.4701371716616958</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9406634036005972</v>
+        <v>-0.54048570004937879</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>5.3430292237151171</v>
+        <v>0.98536978404206543</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8102749798657998</v>
+        <v>6.7834804608351735</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3266081200464432</v>
+        <v>5.6871953111311218</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9876909205319624</v>
+        <v>-0.96337657582994485</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9708765926669543</v>
+        <v>1.2894515306346515</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1596460839860478</v>
+        <v>5.5393681805461092</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5885302457819188</v>
+        <v>1.1617795481698474</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.7393574656273496</v>
+        <v>4.7229008068354617E-3</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1044334480707896</v>
+        <v>4.9991597346338574</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1634084172039998</v>
+        <v>4.2549138785529257</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25792601064294418</v>
+        <v>-2.4390570889391157</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28111008706534202</v>
+        <v>6.109436690978395</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7587356685737925</v>
+        <v>2.3741687657774007</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.4119771573353095</v>
+        <v>5.0251684801028116</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.96817959910065099</v>
+        <v>6.4612708334788955</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5555857668224675</v>
+        <v>-2.5359178279431367</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.0181024646597718</v>
+        <v>6.2246286223385177</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6864945614180336</v>
+        <v>-9.7322114657946823E-2</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>4.34290115053318</v>
+        <v>1.0651658541582609</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>5.3878937830671578</v>
+        <v>3.8332529748901658</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0441557796872658</v>
+        <v>-2.9224340591288129</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7667172703636567</v>
+        <v>0.64495308845509758</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.0645156331442736</v>
+        <v>-2.9143513147846152</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.1669266286678621</v>
+        <v>-2.7680054279858517</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.75091847844858828</v>
+        <v>2.9838241422893077</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3590772704280898</v>
+        <v>-1.44859578382401</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7904364590145221</v>
+        <v>-1.6023856619669392</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.23740052303746495</v>
+        <v>-0.35657585818196047</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1235878070951681</v>
+        <v>0.96408597979283872</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5885208563392226</v>
+        <v>-2.9769991979152906</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.4852863473141715</v>
+        <v>6.9398191489824583</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>2.23093229733621</v>
+        <v>1.6250018914565274</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1247002971110529</v>
+        <v>7.4002135201705066E-3</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8598321452089017</v>
+        <v>-1.8319262321134451</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3275880120470234</v>
+        <v>0.27344216486341288</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4409099865772443</v>
+        <v>4.900218264559439</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8310325290092972</v>
+        <v>2.5157551620877534</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.7030691728865435E-4</v>
+        <v>-0.99673381535887184</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9537891415861317</v>
+        <v>3.4373185172766512</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.5453519145889589</v>
+        <v>1.309757543942573</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6089670061859964</v>
+        <v>5.6106641251253784</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59740640386725818</v>
+        <v>1.446889181903857</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>2.85431599533133</v>
+        <v>-1.4996677434866852</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.34167523380348497</v>
+        <v>6.3146755765392726</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1216033244504446</v>
+        <v>1.6841063251739268</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0723039659851663</v>
+        <v>-2.8910792322805485</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.6291089723033352</v>
+        <v>1.7492799515614301</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3485443937382868</v>
+        <v>0.71621271807293319</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0663511460145028</v>
+        <v>-0.69665699078526888</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9370292595195684</v>
+        <v>1.6594139776781827</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3634381375583997</v>
+        <v>3.7152334270779708</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.5851720603501178</v>
+        <v>2.6450963412880375</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.88119851900638135</v>
+        <v>5.1002999894587884</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4315307325970608</v>
+        <v>-1.7868958623109317</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>6.837984910085158</v>
+        <v>-2.8086647602023627</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>3.634366975405765</v>
+        <v>-0.80987443878919407</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>8.0571672091527713E-2</v>
+        <v>-0.75532098489913446</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.49213136335741803</v>
+        <v>3.1318548711026999</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.26063049627387525</v>
+        <v>3.0221205129459552</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.7118906519350647</v>
+        <v>-1.9380326143316058</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.932016741343044</v>
+        <v>-5.6773514995914098E-2</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.9812558689461164</v>
+        <v>-2.6992939888048402</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.4313682567149137</v>
+        <v>5.5706885462778324</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8693087462373734</v>
+        <v>4.7471161504895729</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.4694845624358015</v>
+        <v>-2.4505437332341113</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2210952466808447</v>
+        <v>-5.2836584598516367E-2</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.6867330721825575</v>
+        <v>-2.3360452693119598</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>5.8713122705984784</v>
+        <v>4.9576098145688681</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.2154006166343998</v>
+        <v>5.2891631805456623</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2246554637569256</v>
+        <v>6.0474552282226242</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12656769523761868</v>
+        <v>-0.2032099343413325</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.16470888122400007</v>
+        <v>5.8694502247522458</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.72117117760458083</v>
+        <v>-1.0947383473644008</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>3.150665402039758</v>
+        <v>2.2842866641609305</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.85331782510886267</v>
+        <v>5.6847533585004175</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.567220543354902</v>
+        <v>4.5571453641889628</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0029581792862601</v>
+        <v>1.8126536808966893</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7579398330084466</v>
+        <v>-2.5849819341402198</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>1.367454760296595</v>
+        <v>-1.2841927192588183</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.85964544556675193</v>
+        <v>-0.56820485015291666</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>5.4169370529491978</v>
+        <v>5.7572117929549496</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>1.8783284480250657</v>
+        <v>-2.2305324750765196</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.32608686019933586</v>
+        <v>-2.0640527601216094</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7955221563897279</v>
+        <v>6.3315409365564115</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.5564007385151419</v>
+        <v>6.8737537734676053</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change to using vigilant deflation
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/BulgeChaserTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/BulgeChaserTest.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-240" yWindow="1605" windowWidth="19440" windowHeight="11040" activeTab="3"/>
+    <workbookView xWindow="-240" yWindow="1605" windowWidth="19440" windowHeight="11040" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="By Diag 6x6" sheetId="1" r:id="rId1"/>
     <sheet name="By Diag 4x4" sheetId="2" r:id="rId2"/>
     <sheet name="By Diag 5x5 in 7x7" sheetId="5" r:id="rId3"/>
     <sheet name="Full 6x6" sheetId="4" r:id="rId4"/>
-    <sheet name="rand" sheetId="3" r:id="rId5"/>
+    <sheet name="Full 6x6 Deflated At 4" sheetId="6" r:id="rId5"/>
+    <sheet name="rand" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="31">
   <si>
     <t>#1</t>
   </si>
@@ -5083,8 +5084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="AA12" sqref="AA12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7934,10 +7935,2864 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="39" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.1299190577623675</v>
+      </c>
+      <c r="B3">
+        <v>2.7864701917357149</v>
+      </c>
+      <c r="C3">
+        <v>2.0306046292172626</v>
+      </c>
+      <c r="D3">
+        <v>3.3256295562164375</v>
+      </c>
+      <c r="E3">
+        <v>3.928469375483683</v>
+      </c>
+      <c r="F3">
+        <v>-1.3341115715941216</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <f>SQRT(A4*A4+A5*A5)</f>
+        <v>2.744554587277102</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <f>A4/I3</f>
+        <v>0.96762608494178581</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <f t="array" ref="AA3:AF8">MMULT(T3:Y8,MMULT(M3:R8,A3:F8))</f>
+        <v>4.1299190577623675</v>
+      </c>
+      <c r="AB3">
+        <v>2.7864701917357149</v>
+      </c>
+      <c r="AC3">
+        <v>2.0306046292172626</v>
+      </c>
+      <c r="AD3">
+        <v>3.3256295562164375</v>
+      </c>
+      <c r="AE3">
+        <v>3.928469375483683</v>
+      </c>
+      <c r="AF3">
+        <v>-1.3341115715941216</v>
+      </c>
+      <c r="AH3">
+        <f t="array" ref="AH3:AM8">MMULT(MMULT(AA3:AF8,TRANSPOSE(M3:R8)),TRANSPOSE(T3:Y8))</f>
+        <v>4.1299190577623675</v>
+      </c>
+      <c r="AI3">
+        <v>3.9757730909445179</v>
+      </c>
+      <c r="AJ3">
+        <v>2.6681379619211762</v>
+      </c>
+      <c r="AK3">
+        <v>0.1478221238082178</v>
+      </c>
+      <c r="AL3">
+        <v>3.928469375483683</v>
+      </c>
+      <c r="AM3">
+        <v>-1.3341115715941216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2.6557026101959611</v>
+      </c>
+      <c r="B4">
+        <v>-0.11968845256554328</v>
+      </c>
+      <c r="C4">
+        <v>-1.80391156027716</v>
+      </c>
+      <c r="D4">
+        <v>0.30173185395631119</v>
+      </c>
+      <c r="E4">
+        <v>0.66926435268965845</v>
+      </c>
+      <c r="F4">
+        <v>-0.55375222781482059</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <f>A5/I3</f>
+        <v>-0.25238811331010003</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f>K3</f>
+        <v>0.96762608494178581</v>
+      </c>
+      <c r="O4">
+        <f>K4</f>
+        <v>-0.25238811331010003</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <f>K6</f>
+        <v>0.57956645411391883</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <f>K7</f>
+        <v>0.81492498137302105</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>4.7355304431364402</v>
+      </c>
+      <c r="AB4">
+        <v>-2.8636438406405942</v>
+      </c>
+      <c r="AC4">
+        <v>2.7594460288685854</v>
+      </c>
+      <c r="AD4">
+        <v>-1.5475349035575443</v>
+      </c>
+      <c r="AE4">
+        <v>0.56593459470652507</v>
+      </c>
+      <c r="AF4">
+        <v>-1.567462886617184</v>
+      </c>
+      <c r="AH4">
+        <v>4.7355304431364402</v>
+      </c>
+      <c r="AI4">
+        <v>-3.2707065367281309</v>
+      </c>
+      <c r="AJ4">
+        <v>1.947362291390899</v>
+      </c>
+      <c r="AK4">
+        <v>1.9287616666345628</v>
+      </c>
+      <c r="AL4">
+        <v>0.56593459470652507</v>
+      </c>
+      <c r="AM4">
+        <v>-1.567462886617184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-0.69269295415944798</v>
+      </c>
+      <c r="B5">
+        <v>4.8981743369651554</v>
+      </c>
+      <c r="C5">
+        <v>0.96551991318403241</v>
+      </c>
+      <c r="D5">
+        <v>1.1051202838375689</v>
+      </c>
+      <c r="E5">
+        <v>-0.86610480005677681</v>
+      </c>
+      <c r="F5">
+        <v>0.68202546678859566</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f>-O4</f>
+        <v>0.25238811331010003</v>
+      </c>
+      <c r="O5">
+        <f>N4</f>
+        <v>0.96762608494178581</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>1.1102230246251565E-16</v>
+      </c>
+      <c r="AB5">
+        <v>4.7093933143118978</v>
+      </c>
+      <c r="AC5">
+        <v>0.47897641825096698</v>
+      </c>
+      <c r="AD5">
+        <v>1.1454967469850938</v>
+      </c>
+      <c r="AE5">
+        <v>-0.66915122954717887</v>
+      </c>
+      <c r="AF5">
+        <v>0.52018515223979545</v>
+      </c>
+      <c r="AH5">
+        <v>1.1102230246251565E-16</v>
+      </c>
+      <c r="AI5">
+        <v>3.5044761258140467</v>
+      </c>
+      <c r="AJ5">
+        <v>1.6520649698060015</v>
+      </c>
+      <c r="AK5">
+        <v>-2.9511514726660208</v>
+      </c>
+      <c r="AL5">
+        <v>-0.66915122954717887</v>
+      </c>
+      <c r="AM5">
+        <v>0.52018515223979545</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3.8591020581643383</v>
+      </c>
+      <c r="B6">
+        <v>-2.5524292049923321</v>
+      </c>
+      <c r="C6">
+        <v>4.8008323897154961</v>
+      </c>
+      <c r="D6">
+        <v>-1.9082676681357242</v>
+      </c>
+      <c r="E6">
+        <v>7.8435013270618192E-2</v>
+      </c>
+      <c r="F6">
+        <v>-1.4199502016946737</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f>SQRT(I3*I3+A6*A6)</f>
+        <v>4.7355304431364411</v>
+      </c>
+      <c r="J6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <f>I3/I6</f>
+        <v>0.57956645411391883</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <f>-W4</f>
+        <v>-0.81492498137302105</v>
+      </c>
+      <c r="V6">
+        <f>T4</f>
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <f>U4</f>
+        <v>0.57956645411391883</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>-4.4408920985006262E-16</v>
+      </c>
+      <c r="AB6">
+        <v>-0.37747923460098542</v>
+      </c>
+      <c r="AC6">
+        <v>4.4034482463994902</v>
+      </c>
+      <c r="AD6">
+        <v>-1.1165981244883969</v>
+      </c>
+      <c r="AE6">
+        <v>-0.66042336139715618</v>
+      </c>
+      <c r="AF6">
+        <v>-0.2460210334865871</v>
+      </c>
+      <c r="AH6">
+        <v>-4.4408920985006262E-16</v>
+      </c>
+      <c r="AI6">
+        <v>-1.7657528303690404</v>
+      </c>
+      <c r="AJ6">
+        <v>4.1656201150726275</v>
+      </c>
+      <c r="AK6">
+        <v>0.55620535940489479</v>
+      </c>
+      <c r="AL6">
+        <v>-0.66042336139715618</v>
+      </c>
+      <c r="AM6">
+        <v>-0.2460210334865871</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f>POWER(10,-15)</f>
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="E7">
+        <v>1.593627460433078</v>
+      </c>
+      <c r="F7">
+        <v>3.4960354799137559</v>
+      </c>
+      <c r="J7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <f>A6/I6</f>
+        <v>0.81492498137302105</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="AE7">
+        <v>1.593627460433078</v>
+      </c>
+      <c r="AF7">
+        <v>3.4960354799137559</v>
+      </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
+        <v>8.1492498137302111E-16</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>5.7956645411391891E-16</v>
+      </c>
+      <c r="AL7">
+        <v>1.593627460433078</v>
+      </c>
+      <c r="AM7">
+        <v>3.4960354799137559</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>4.2308444229492856</v>
+      </c>
+      <c r="F8">
+        <v>3.4350466320112147</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>4.2308444229492856</v>
+      </c>
+      <c r="AF8">
+        <v>3.4350466320112147</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>4.2308444229492856</v>
+      </c>
+      <c r="AM8">
+        <v>3.4350466320112147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="M11" t="s">
+        <v>7</v>
+      </c>
+      <c r="T11" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f>AA3</f>
+        <v>4.1299190577623675</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" ref="B12:F13" si="0">AB3</f>
+        <v>2.7864701917357149</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>2.0306046292172626</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3256295562164375</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>3.928469375483683</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.3341115715941216</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <f>SQRT(B14*B14+B15*B15)</f>
+        <v>3.9241860269815074</v>
+      </c>
+      <c r="J12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <f>B14/I12</f>
+        <v>0.89304536067310181</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="1">
+        <f t="array" ref="AA12:AF17">MMULT(T12:Y17,MMULT(M12:R17,AH3:AM8))</f>
+        <v>4.1299190577623675</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>3.9757730909445179</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>2.6681379619211762</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>0.1478221238082178</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>3.928469375483683</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>-1.3341115715941216</v>
+      </c>
+      <c r="AH12">
+        <f t="array" ref="AH12:AM17">MMULT(MMULT(AA12:AF17,TRANSPOSE(M12:R17)), TRANSPOSE(T12:Y17))</f>
+        <v>4.1299190577623675</v>
+      </c>
+      <c r="AI12">
+        <v>3.9757730909445179</v>
+      </c>
+      <c r="AJ12">
+        <v>2.3162532030666712</v>
+      </c>
+      <c r="AK12">
+        <v>1.3325849554213987</v>
+      </c>
+      <c r="AL12">
+        <v>3.9284693754836826</v>
+      </c>
+      <c r="AM12">
+        <v>-1.3341115715941216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <f>AA4</f>
+        <v>4.7355304431364402</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>-2.8636438406405942</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7594460288685854</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.5475349035575443</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.56593459470652507</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.567462886617184</v>
+      </c>
+      <c r="J13" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13">
+        <f>B15/I12</f>
+        <v>-0.44996664740872677</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>4.7355304431364402</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>-3.2707065367281309</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>1.947362291390899</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>1.9287616666345628</v>
+      </c>
+      <c r="AE13" s="1">
+        <v>0.56593459470652507</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>-1.567462886617184</v>
+      </c>
+      <c r="AH13">
+        <v>4.7355304431364402</v>
+      </c>
+      <c r="AI13">
+        <v>-3.2707065367281309</v>
+      </c>
+      <c r="AJ13">
+        <v>0.87120443909036105</v>
+      </c>
+      <c r="AK13">
+        <v>2.598719739779455</v>
+      </c>
+      <c r="AL13">
+        <v>0.56593459470652485</v>
+      </c>
+      <c r="AM13">
+        <v>-1.567462886617184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" ref="A14:F17" si="1">AH5</f>
+        <v>1.1102230246251565E-16</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>3.5044761258140467</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>1.6520649698060015</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>-2.9511514726660208</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>-0.66915122954717887</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0.52018515223979545</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>K12</f>
+        <v>0.89304536067310181</v>
+      </c>
+      <c r="P14">
+        <f>K13</f>
+        <v>-0.44996664740872677</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <f>K15</f>
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <f>K16</f>
+        <v>2.0766726545832568E-16</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>2.9897328505201868E-16</v>
+      </c>
+      <c r="AB14">
+        <v>3.924186026981507</v>
+      </c>
+      <c r="AC14">
+        <v>-0.39902116074178706</v>
+      </c>
+      <c r="AD14">
+        <v>-2.8857859921501685</v>
+      </c>
+      <c r="AE14">
+        <v>-0.3004139153375292</v>
+      </c>
+      <c r="AF14">
+        <v>0.57525019652877096</v>
+      </c>
+      <c r="AH14">
+        <v>2.9897328505201868E-16</v>
+      </c>
+      <c r="AI14">
+        <v>3.924186026981507</v>
+      </c>
+      <c r="AJ14">
+        <v>0.94216345161602855</v>
+      </c>
+      <c r="AK14">
+        <v>-2.7566840061292526</v>
+      </c>
+      <c r="AL14">
+        <v>-0.30041391533752942</v>
+      </c>
+      <c r="AM14">
+        <v>0.57525019652877096</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>-4.4408920985006262E-16</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>-1.7657528303690404</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>4.1656201150726275</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>0.55620535940489479</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>-0.66042336139715618</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>-0.2460210334865871</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <f>SQRT(I12*I12+B16*B16)</f>
+        <v>3.9241860269815074</v>
+      </c>
+      <c r="J15" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <f>I12/I15</f>
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>-P14</f>
+        <v>0.44996664740872677</v>
+      </c>
+      <c r="P15">
+        <f>O14</f>
+        <v>0.89304536067310181</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>-3.4663547535492615E-16</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>4.4634618538571686</v>
+      </c>
+      <c r="AD15">
+        <v>-0.8312031183527997</v>
+      </c>
+      <c r="AE15">
+        <v>-0.89088375434463707</v>
+      </c>
+      <c r="AF15">
+        <v>1.4358026401940449E-2</v>
+      </c>
+      <c r="AH15">
+        <v>-3.4663547535492615E-16</v>
+      </c>
+      <c r="AI15">
+        <v>0</v>
+      </c>
+      <c r="AJ15">
+        <v>4.3600875816093954</v>
+      </c>
+      <c r="AK15">
+        <v>1.2661068775948678</v>
+      </c>
+      <c r="AL15">
+        <v>-0.89088375434463796</v>
+      </c>
+      <c r="AM15">
+        <v>1.4358026401940449E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>8.1492498137302111E-16</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>5.7956645411391891E-16</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>1.593627460433078</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>3.4960354799137559</v>
+      </c>
+      <c r="J16" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <f>B16/I15</f>
+        <v>2.0766726545832568E-16</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <f>-X14</f>
+        <v>-2.0766726545832568E-16</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <f>V14</f>
+        <v>1</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>-6.2086964551845232E-32</v>
+      </c>
+      <c r="AB16">
+        <v>9.8607613152626476E-32</v>
+      </c>
+      <c r="AC16">
+        <v>8.2863633311253934E-17</v>
+      </c>
+      <c r="AD16">
+        <v>1.1788497398016858E-15</v>
+      </c>
+      <c r="AE16">
+        <v>1.593627460433078</v>
+      </c>
+      <c r="AF16">
+        <v>3.4960354799137559</v>
+      </c>
+      <c r="AH16">
+        <v>-6.2086964551845232E-32</v>
+      </c>
+      <c r="AI16">
+        <v>9.8607613152626476E-32</v>
+      </c>
+      <c r="AJ16">
+        <v>-1.2549782505264859E-16</v>
+      </c>
+      <c r="AK16">
+        <v>1.0900521623337596E-15</v>
+      </c>
+      <c r="AL16">
+        <v>1.593627460433078</v>
+      </c>
+      <c r="AM16">
+        <v>3.4960354799137559</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>4.2308444229492856</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>3.4350466320112147</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>1</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>4.2308444229492856</v>
+      </c>
+      <c r="AF17">
+        <v>3.4350466320112147</v>
+      </c>
+      <c r="AH17">
+        <v>0</v>
+      </c>
+      <c r="AI17">
+        <v>0</v>
+      </c>
+      <c r="AJ17">
+        <v>8.7860789189348605E-16</v>
+      </c>
+      <c r="AK17">
+        <v>0</v>
+      </c>
+      <c r="AL17">
+        <v>4.2308444229492856</v>
+      </c>
+      <c r="AM17">
+        <v>3.4350466320112147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="M20" t="s">
+        <v>14</v>
+      </c>
+      <c r="T20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <f>A12</f>
+        <v>4.1299190577623675</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" ref="B21:F22" si="2">B12</f>
+        <v>2.7864701917357149</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="2"/>
+        <v>2.0306046292172626</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="2"/>
+        <v>3.3256295562164375</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="2"/>
+        <v>3.928469375483683</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.3341115715941216</v>
+      </c>
+      <c r="H21" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <f>SQRT(C24*C24+C25*C25)</f>
+        <v>4.3600875816093954</v>
+      </c>
+      <c r="J21" t="s">
+        <v>2</v>
+      </c>
+      <c r="K21">
+        <f>C24/I21</f>
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="AA21">
+        <f t="array" ref="AA21:AF26">MMULT(T21:Y26,MMULT(M21:R26,AH12:AM17))</f>
+        <v>4.1299190577623675</v>
+      </c>
+      <c r="AB21">
+        <v>3.9757730909445179</v>
+      </c>
+      <c r="AC21">
+        <v>2.3162532030666712</v>
+      </c>
+      <c r="AD21">
+        <v>1.3325849554213987</v>
+      </c>
+      <c r="AE21">
+        <v>3.9284693754836826</v>
+      </c>
+      <c r="AF21">
+        <v>-1.3341115715941216</v>
+      </c>
+      <c r="AH21">
+        <f t="array" ref="AH21:AM26">MMULT(MMULT(AA21:AF26,TRANSPOSE(M21:R26)), TRANSPOSE(T21:Y26))</f>
+        <v>4.1299190577623675</v>
+      </c>
+      <c r="AI21">
+        <v>3.9757730909445179</v>
+      </c>
+      <c r="AJ21">
+        <v>2.3162532030666712</v>
+      </c>
+      <c r="AK21">
+        <v>1.3325849554213982</v>
+      </c>
+      <c r="AL21">
+        <v>3.9284693754836826</v>
+      </c>
+      <c r="AM21">
+        <v>-1.3341115715941219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <f>A13</f>
+        <v>4.7355304431364402</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="2"/>
+        <v>-2.8636438406405942</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="2"/>
+        <v>2.7594460288685854</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.5475349035575443</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="2"/>
+        <v>0.56593459470652507</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.567462886617184</v>
+      </c>
+      <c r="J22" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22">
+        <f>C25/I21</f>
+        <v>-2.8783326642792994E-17</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="AA22">
+        <v>4.7355304431364402</v>
+      </c>
+      <c r="AB22">
+        <v>-3.2707065367281309</v>
+      </c>
+      <c r="AC22">
+        <v>0.87120443909036105</v>
+      </c>
+      <c r="AD22">
+        <v>2.598719739779455</v>
+      </c>
+      <c r="AE22">
+        <v>0.56593459470652485</v>
+      </c>
+      <c r="AF22">
+        <v>-1.567462886617184</v>
+      </c>
+      <c r="AH22">
+        <v>4.7355304431364402</v>
+      </c>
+      <c r="AI22">
+        <v>-3.2707065367281309</v>
+      </c>
+      <c r="AJ22">
+        <v>0.87120443909036105</v>
+      </c>
+      <c r="AK22">
+        <v>2.5987197397794546</v>
+      </c>
+      <c r="AL22">
+        <v>0.56593459470652496</v>
+      </c>
+      <c r="AM22">
+        <v>-1.5674628866171845</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <f>AA14</f>
+        <v>2.9897328505201868E-16</v>
+      </c>
+      <c r="B23" s="1">
+        <f t="shared" ref="B23:F23" si="3">AB14</f>
+        <v>3.924186026981507</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.39902116074178706</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="3"/>
+        <v>-2.8857859921501685</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.3004139153375292</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="3"/>
+        <v>0.57525019652877096</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>2.9897328505201868E-16</v>
+      </c>
+      <c r="AB23">
+        <v>3.924186026981507</v>
+      </c>
+      <c r="AC23">
+        <v>0.94216345161602855</v>
+      </c>
+      <c r="AD23">
+        <v>-2.7566840061292526</v>
+      </c>
+      <c r="AE23">
+        <v>-0.30041391533752942</v>
+      </c>
+      <c r="AF23">
+        <v>0.57525019652877096</v>
+      </c>
+      <c r="AH23">
+        <v>2.9897328505201868E-16</v>
+      </c>
+      <c r="AI23">
+        <v>3.924186026981507</v>
+      </c>
+      <c r="AJ23">
+        <v>0.94216345161602855</v>
+      </c>
+      <c r="AK23">
+        <v>-2.7566840061292526</v>
+      </c>
+      <c r="AL23">
+        <v>-0.30041391533752948</v>
+      </c>
+      <c r="AM23">
+        <v>0.57525019652877152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" ref="A24:F26" si="4">AH15</f>
+        <v>-3.4663547535492615E-16</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="4"/>
+        <v>4.3600875816093954</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="4"/>
+        <v>1.2661068775948678</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="4"/>
+        <v>-0.89088375434463796</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="4"/>
+        <v>1.4358026401940449E-2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <f>SQRT(I21*I21+C26*C26)</f>
+        <v>4.3600875816093954</v>
+      </c>
+      <c r="J24" t="s">
+        <v>2</v>
+      </c>
+      <c r="K24">
+        <f>I21/I24</f>
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <f>K21</f>
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <f>K22</f>
+        <v>-2.8783326642792994E-17</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <f>K24</f>
+        <v>1</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <f>K25</f>
+        <v>2.015115236674155E-16</v>
+      </c>
+      <c r="AA24">
+        <v>-3.4663547535492615E-16</v>
+      </c>
+      <c r="AB24">
+        <v>-2.8382551388382185E-48</v>
+      </c>
+      <c r="AC24">
+        <v>4.3600875816093954</v>
+      </c>
+      <c r="AD24">
+        <v>1.2661068775948678</v>
+      </c>
+      <c r="AE24">
+        <v>-0.89088375434463707</v>
+      </c>
+      <c r="AF24">
+        <v>1.4358026401941041E-2</v>
+      </c>
+      <c r="AH24">
+        <v>-3.4663547535492615E-16</v>
+      </c>
+      <c r="AI24">
+        <v>-2.8382551388382185E-48</v>
+      </c>
+      <c r="AJ24">
+        <v>4.3600875816093954</v>
+      </c>
+      <c r="AK24">
+        <v>1.2661068775948678</v>
+      </c>
+      <c r="AL24">
+        <v>-0.89088375434463707</v>
+      </c>
+      <c r="AM24">
+        <v>1.4358026401940786E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="4"/>
+        <v>-6.2086964551845232E-32</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="4"/>
+        <v>9.8607613152626476E-32</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="4"/>
+        <v>-1.2549782505264859E-16</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="4"/>
+        <v>1.0900521623337596E-15</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="4"/>
+        <v>1.593627460433078</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="4"/>
+        <v>3.4960354799137559</v>
+      </c>
+      <c r="J25" t="s">
+        <v>3</v>
+      </c>
+      <c r="K25">
+        <f>C26/I24</f>
+        <v>2.015115236674155E-16</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <f>-Q24</f>
+        <v>2.8783326642792994E-17</v>
+      </c>
+      <c r="Q25">
+        <f>P24</f>
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <v>1</v>
+      </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <v>-7.2064286664965889E-32</v>
+      </c>
+      <c r="AB25">
+        <v>9.8607613152626476E-32</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <v>1.1264949301562595E-15</v>
+      </c>
+      <c r="AE25">
+        <v>1.593627460433078</v>
+      </c>
+      <c r="AF25">
+        <v>3.4960354799137559</v>
+      </c>
+      <c r="AH25">
+        <v>-7.2064286664965889E-32</v>
+      </c>
+      <c r="AI25">
+        <v>9.8607613152626476E-32</v>
+      </c>
+      <c r="AJ25">
+        <v>0</v>
+      </c>
+      <c r="AK25">
+        <v>1.7851164667684545E-15</v>
+      </c>
+      <c r="AL25">
+        <v>1.593627460433078</v>
+      </c>
+      <c r="AM25">
+        <v>3.4960354799137559</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="4"/>
+        <v>8.7860789189348605E-16</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="4"/>
+        <v>4.2308444229492856</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="4"/>
+        <v>3.4350466320112147</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <f>-Y24</f>
+        <v>-2.015115236674155E-16</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <f>W24</f>
+        <v>1</v>
+      </c>
+      <c r="AA26">
+        <v>6.9851042795950027E-32</v>
+      </c>
+      <c r="AB26">
+        <v>5.7194111758416132E-64</v>
+      </c>
+      <c r="AC26">
+        <v>0</v>
+      </c>
+      <c r="AD26">
+        <v>-2.5513512602993574E-16</v>
+      </c>
+      <c r="AE26">
+        <v>4.2308444229492856</v>
+      </c>
+      <c r="AF26">
+        <v>3.4350466320112147</v>
+      </c>
+      <c r="AH26">
+        <v>6.9851042795950027E-32</v>
+      </c>
+      <c r="AI26">
+        <v>5.7194111758416132E-64</v>
+      </c>
+      <c r="AJ26">
+        <v>0</v>
+      </c>
+      <c r="AK26">
+        <v>3.1528857765467975E-16</v>
+      </c>
+      <c r="AL26">
+        <v>4.2308444229492856</v>
+      </c>
+      <c r="AM26">
+        <v>3.4350466320112147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="M29" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <f>A21</f>
+        <v>4.1299190577623675</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" ref="B30:F30" si="5">B21</f>
+        <v>2.7864701917357149</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="5"/>
+        <v>2.0306046292172626</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="5"/>
+        <v>3.3256295562164375</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="5"/>
+        <v>3.928469375483683</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="5"/>
+        <v>-1.3341115715941216</v>
+      </c>
+      <c r="H30" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <f>SQRT(D34*D34+D35*D35)</f>
+        <v>1.8127458970102239E-15</v>
+      </c>
+      <c r="J30" t="s">
+        <v>2</v>
+      </c>
+      <c r="K30">
+        <f>D34/I30</f>
+        <v>0.98475824422643077</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="AA30">
+        <f t="array" ref="AA30:AF35">MMULT(M30:R35,AH21:AM26)</f>
+        <v>4.1299190577623675</v>
+      </c>
+      <c r="AB30">
+        <v>3.9757730909445179</v>
+      </c>
+      <c r="AC30">
+        <v>2.3162532030666712</v>
+      </c>
+      <c r="AD30">
+        <v>1.3325849554213982</v>
+      </c>
+      <c r="AE30">
+        <v>3.9284693754836826</v>
+      </c>
+      <c r="AF30">
+        <v>-1.3341115715941219</v>
+      </c>
+      <c r="AH30">
+        <f t="array" ref="AH30:AM35">MMULT(AA30:AF35,TRANSPOSE(M30:R35))</f>
+        <v>4.1299190577623675</v>
+      </c>
+      <c r="AI30">
+        <v>3.9757730909445179</v>
+      </c>
+      <c r="AJ30">
+        <v>2.3162532030666712</v>
+      </c>
+      <c r="AK30">
+        <v>1.3325849554213982</v>
+      </c>
+      <c r="AL30">
+        <v>3.6365522836948219</v>
+      </c>
+      <c r="AM30">
+        <v>-1.9970510277728182</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <f t="shared" ref="A31:F32" si="6">A22</f>
+        <v>4.7355304431364402</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="6"/>
+        <v>-2.8636438406405942</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="6"/>
+        <v>2.7594460288685854</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="6"/>
+        <v>-1.5475349035575443</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="6"/>
+        <v>0.56593459470652507</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="6"/>
+        <v>-1.567462886617184</v>
+      </c>
+      <c r="J31" t="s">
+        <v>3</v>
+      </c>
+      <c r="K31">
+        <f>D35/I30</f>
+        <v>0.17392872226310796</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="AA31">
+        <v>4.7355304431364402</v>
+      </c>
+      <c r="AB31">
+        <v>-3.2707065367281309</v>
+      </c>
+      <c r="AC31">
+        <v>0.87120443909036105</v>
+      </c>
+      <c r="AD31">
+        <v>2.5987197397794546</v>
+      </c>
+      <c r="AE31">
+        <v>0.56593459470652496</v>
+      </c>
+      <c r="AF31">
+        <v>-1.5674628866171845</v>
+      </c>
+      <c r="AH31">
+        <v>4.7355304431364402</v>
+      </c>
+      <c r="AI31">
+        <v>-3.2707065367281309</v>
+      </c>
+      <c r="AJ31">
+        <v>0.87120443909036105</v>
+      </c>
+      <c r="AK31">
+        <v>2.5987197397794546</v>
+      </c>
+      <c r="AL31">
+        <v>0.28468194076602443</v>
+      </c>
+      <c r="AM31">
+        <v>-1.6420042810570272</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <f t="shared" si="6"/>
+        <v>2.9897328505201868E-16</v>
+      </c>
+      <c r="B32" s="1">
+        <f t="shared" si="6"/>
+        <v>3.924186026981507</v>
+      </c>
+      <c r="C32" s="1">
+        <f t="shared" si="6"/>
+        <v>-0.39902116074178706</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="6"/>
+        <v>-2.8857859921501685</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="6"/>
+        <v>-0.3004139153375292</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="6"/>
+        <v>0.57525019652877096</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="AA32">
+        <v>2.9897328505201868E-16</v>
+      </c>
+      <c r="AB32">
+        <v>3.924186026981507</v>
+      </c>
+      <c r="AC32">
+        <v>0.94216345161602855</v>
+      </c>
+      <c r="AD32">
+        <v>-2.7566840061292526</v>
+      </c>
+      <c r="AE32">
+        <v>-0.30041391533752948</v>
+      </c>
+      <c r="AF32">
+        <v>0.57525019652877152</v>
+      </c>
+      <c r="AH32">
+        <v>2.9897328505201868E-16</v>
+      </c>
+      <c r="AI32">
+        <v>3.924186026981507</v>
+      </c>
+      <c r="AJ32">
+        <v>0.94216345161602855</v>
+      </c>
+      <c r="AK32">
+        <v>-2.7566840061292526</v>
+      </c>
+      <c r="AL32">
+        <v>-0.19578254814512219</v>
+      </c>
+      <c r="AM32">
+        <v>0.61873298196929627</v>
+      </c>
+    </row>
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <f>AA24</f>
+        <v>-3.4663547535492615E-16</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" ref="B33:F33" si="7">AB24</f>
+        <v>-2.8382551388382185E-48</v>
+      </c>
+      <c r="C33" s="1">
+        <f t="shared" si="7"/>
+        <v>4.3600875816093954</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="7"/>
+        <v>1.2661068775948678</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="7"/>
+        <v>-0.89088375434463707</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="7"/>
+        <v>1.4358026401941041E-2</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="AA33">
+        <v>-3.4663547535492615E-16</v>
+      </c>
+      <c r="AB33">
+        <v>-2.8382551388382185E-48</v>
+      </c>
+      <c r="AC33">
+        <v>4.3600875816093954</v>
+      </c>
+      <c r="AD33">
+        <v>1.2661068775948678</v>
+      </c>
+      <c r="AE33">
+        <v>-0.89088375434463707</v>
+      </c>
+      <c r="AF33">
+        <v>1.4358026401940786E-2</v>
+      </c>
+      <c r="AH33">
+        <v>-3.4663547535492615E-16</v>
+      </c>
+      <c r="AI33">
+        <v>-2.8382551388382185E-48</v>
+      </c>
+      <c r="AJ33">
+        <v>4.3600875816093954</v>
+      </c>
+      <c r="AK33">
+        <v>1.2661068775948678</v>
+      </c>
+      <c r="AL33">
+        <v>-0.87480784855196614</v>
+      </c>
+      <c r="AM33">
+        <v>0.16908945794825522</v>
+      </c>
+    </row>
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" ref="A34:F35" si="8">AH25</f>
+        <v>-7.2064286664965889E-32</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="8"/>
+        <v>9.8607613152626476E-32</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="8"/>
+        <v>1.7851164667684545E-15</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="8"/>
+        <v>1.593627460433078</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="8"/>
+        <v>3.4960354799137559</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <f>K30</f>
+        <v>0.98475824422643077</v>
+      </c>
+      <c r="R34">
+        <f>K31</f>
+        <v>0.17392872226310796</v>
+      </c>
+      <c r="AA34">
+        <v>-5.8816797785376744E-32</v>
+      </c>
+      <c r="AB34">
+        <v>9.710465999553955E-32</v>
+      </c>
+      <c r="AC34">
+        <v>0</v>
+      </c>
+      <c r="AD34">
+        <v>1.8127458970102239E-15</v>
+      </c>
+      <c r="AE34">
+        <v>2.3052031444646692</v>
+      </c>
+      <c r="AF34">
+        <v>4.0402030325730802</v>
+      </c>
+      <c r="AH34">
+        <v>-5.8816797785376744E-32</v>
+      </c>
+      <c r="AI34">
+        <v>9.710465999553955E-32</v>
+      </c>
+      <c r="AJ34">
+        <v>0</v>
+      </c>
+      <c r="AK34">
+        <v>1.8127458970102239E-15</v>
+      </c>
+      <c r="AL34">
+        <v>2.9727751522672445</v>
+      </c>
+      <c r="AM34">
+        <v>3.5776822072013292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="8"/>
+        <v>6.9851042795950027E-32</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="8"/>
+        <v>5.7194111758416132E-64</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="8"/>
+        <v>3.1528857765467975E-16</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="8"/>
+        <v>4.2308444229492856</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="8"/>
+        <v>3.4350466320112147</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <f>-R34</f>
+        <v>-0.17392872226310796</v>
+      </c>
+      <c r="R35">
+        <f>Q34</f>
+        <v>0.98475824422643077</v>
+      </c>
+      <c r="AA35">
+        <v>8.1320439561564882E-32</v>
+      </c>
+      <c r="AB35">
+        <v>-1.7150696161051162E-32</v>
+      </c>
+      <c r="AC35">
+        <v>0</v>
+      </c>
+      <c r="AD35">
+        <v>0</v>
+      </c>
+      <c r="AE35">
+        <v>3.8891813375821984</v>
+      </c>
+      <c r="AF35">
+        <v>2.7746295061673871</v>
+      </c>
+      <c r="AH35">
+        <v>8.1320439561564882E-32</v>
+      </c>
+      <c r="AI35">
+        <v>-1.7150696161051162E-32</v>
+      </c>
+      <c r="AJ35">
+        <v>0</v>
+      </c>
+      <c r="AK35">
+        <v>0</v>
+      </c>
+      <c r="AL35">
+        <v>4.312491150236859</v>
+      </c>
+      <c r="AM35">
+        <v>2.0558989401770478</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>6</v>
+      </c>
+      <c r="B38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <f>A30</f>
+        <v>4.1299190577623675</v>
+      </c>
+      <c r="B39" s="1">
+        <f t="shared" ref="B39:F39" si="9">B30</f>
+        <v>2.7864701917357149</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="9"/>
+        <v>2.0306046292172626</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="9"/>
+        <v>3.3256295562164375</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="9"/>
+        <v>3.928469375483683</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="9"/>
+        <v>-1.3341115715941216</v>
+      </c>
+    </row>
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <f t="shared" ref="A40:F42" si="10">A31</f>
+        <v>4.7355304431364402</v>
+      </c>
+      <c r="B40" s="1">
+        <f t="shared" si="10"/>
+        <v>-2.8636438406405942</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" si="10"/>
+        <v>2.7594460288685854</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="10"/>
+        <v>-1.5475349035575443</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="10"/>
+        <v>0.56593459470652507</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="10"/>
+        <v>-1.567462886617184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <f t="shared" si="10"/>
+        <v>2.9897328505201868E-16</v>
+      </c>
+      <c r="B41" s="1">
+        <f t="shared" si="10"/>
+        <v>3.924186026981507</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" si="10"/>
+        <v>-0.39902116074178706</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="10"/>
+        <v>-2.8857859921501685</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="10"/>
+        <v>-0.3004139153375292</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="10"/>
+        <v>0.57525019652877096</v>
+      </c>
+    </row>
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <f t="shared" si="10"/>
+        <v>-3.4663547535492615E-16</v>
+      </c>
+      <c r="B42" s="1">
+        <f t="shared" si="10"/>
+        <v>-2.8382551388382185E-48</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="10"/>
+        <v>4.3600875816093954</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="10"/>
+        <v>1.2661068775948678</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="10"/>
+        <v>-0.89088375434463707</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="10"/>
+        <v>1.4358026401941041E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <f>AA34</f>
+        <v>-5.8816797785376744E-32</v>
+      </c>
+      <c r="B43" s="1">
+        <f t="shared" ref="B43:F43" si="11">AB34</f>
+        <v>9.710465999553955E-32</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" si="11"/>
+        <v>1.8127458970102239E-15</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="11"/>
+        <v>2.3052031444646692</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="11"/>
+        <v>4.0402030325730802</v>
+      </c>
+    </row>
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" ref="A44:F44" si="12">AH35</f>
+        <v>8.1320439561564882E-32</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="12"/>
+        <v>-1.7150696161051162E-32</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="12"/>
+        <v>4.312491150236859</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="12"/>
+        <v>2.0558989401770478</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>6</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f>AH30</f>
+        <v>4.1299190577623675</v>
+      </c>
+      <c r="B48">
+        <f t="shared" ref="B48:F53" si="13">AI30</f>
+        <v>3.9757730909445179</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="13"/>
+        <v>2.3162532030666712</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="13"/>
+        <v>1.3325849554213982</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="13"/>
+        <v>3.6365522836948219</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="13"/>
+        <v>-1.9970510277728182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" ref="A49:A53" si="14">AH31</f>
+        <v>4.7355304431364402</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="13"/>
+        <v>-3.2707065367281309</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="13"/>
+        <v>0.87120443909036105</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="13"/>
+        <v>2.5987197397794546</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="13"/>
+        <v>0.28468194076602443</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="13"/>
+        <v>-1.6420042810570272</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="14"/>
+        <v>2.9897328505201868E-16</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="13"/>
+        <v>3.924186026981507</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="13"/>
+        <v>0.94216345161602855</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="13"/>
+        <v>-2.7566840061292526</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="13"/>
+        <v>-0.19578254814512219</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="13"/>
+        <v>0.61873298196929627</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="14"/>
+        <v>-3.4663547535492615E-16</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="13"/>
+        <v>-2.8382551388382185E-48</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="13"/>
+        <v>4.3600875816093954</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="13"/>
+        <v>1.2661068775948678</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="13"/>
+        <v>-0.87480784855196614</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="13"/>
+        <v>0.16908945794825522</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="14"/>
+        <v>-5.8816797785376744E-32</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="13"/>
+        <v>9.710465999553955E-32</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="13"/>
+        <v>1.8127458970102239E-15</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="13"/>
+        <v>2.9727751522672445</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="13"/>
+        <v>3.5776822072013292</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="14"/>
+        <v>8.1320439561564882E-32</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="13"/>
+        <v>-1.7150696161051162E-32</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="13"/>
+        <v>4.312491150236859</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="13"/>
+        <v>2.0558989401770478</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:H8"/>
+      <selection activeCell="B7" sqref="B7:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7945,799 +10800,799 @@
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND()*10-3</f>
-        <v>-0.38359501537838581</v>
+        <v>6.717733902915608</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:J16" ca="1" si="0">RAND()*10-3</f>
-        <v>0.53848117489840464</v>
+        <v>3.5553225170189355</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.48831023151230069</v>
+        <v>-1.3455434832802577</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3156616284243032</v>
+        <v>-0.86078111444708938</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.6517580557681695</v>
+        <v>-2.5903986715303837</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.0163508720970689</v>
+        <v>3.9040799903836492</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7106287160216156</v>
+        <v>6.8713229854572599</v>
       </c>
       <c r="H1">
         <f ca="1">RAND()*10-3</f>
-        <v>3.5142311047359023</v>
+        <v>5.537832619939886</v>
       </c>
       <c r="I1">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.6079891175597489</v>
+        <v>-0.63129695795774587</v>
       </c>
       <c r="J1">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.456344037716268</v>
+        <v>-2.5733219066366324</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:J19" ca="1" si="1">RAND()*10-3</f>
-        <v>5.2951193027848031</v>
+        <v>5.3137142744978405</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5200264381873776</v>
+        <v>-1.294477673569528</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1332102958984471</v>
+        <v>6.4284650425391998</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2257935668461748</v>
+        <v>6.8465890980057331</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1291768640166957</v>
+        <v>2.2335883838376578</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61551012421407636</v>
+        <v>1.6627188467634024</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5405708457929137</v>
+        <v>2.1009600613241171</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>5.9658745302591676</v>
+        <v>3.2737636037967537</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9818216291691284</v>
+        <v>6.2836902568534114</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2046070007102934</v>
+        <v>3.001569769448861</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.6458359926136874</v>
+        <v>6.9536270364633914</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.36785392506988</v>
+        <v>-2.5968446261309159</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5744061433321797</v>
+        <v>1.8960748893132369</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.933387702138436</v>
+        <v>-1.0673425333504167</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7304806693276644</v>
+        <v>3.1826979898131889</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1195028362955526</v>
+        <v>-1.6641561561528735</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6387680374151614</v>
+        <v>-2.0877019907810319</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.32648985616896375</v>
+        <v>5.2214449870976587</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.35937780381745954</v>
+        <v>-1.0889545063244828</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2525009652220938</v>
+        <v>-1.6522655211059785</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.002649552835851</v>
+        <v>3.8810562379366971</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0197997195020081</v>
+        <v>1.0037221664821736</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5718695463503742</v>
+        <v>4.0065323508529804</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7539967407592769</v>
+        <v>4.6340195465426239</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.32751882526938569</v>
+        <v>-2.6911214632848663</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9529950323954557</v>
+        <v>1.0308740571306636</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.2539824289867203</v>
+        <v>-1.6330784568443986</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4057691896713749</v>
+        <v>6.4944039459488518</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6123699793623629</v>
+        <v>-1.6253598091942962</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1180611212434659</v>
+        <v>5.3183566106361777</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>5.7813273690552158</v>
+        <v>1.2538499771743155</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.43402327160258647</v>
+        <v>3.7598808172630589</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2486709499763737</v>
+        <v>0.5618873252537564</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.2301564807280536</v>
+        <v>3.2853539759938233</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2906208229676039</v>
+        <v>-1.7178395814641474</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3678814229041958</v>
+        <v>3.6797305606328736</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>2.258715959621191</v>
+        <v>5.5016905224139503</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.86226982835533494</v>
+        <v>-2.5894509858853683</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.350088078025351</v>
+        <v>1.8385287211429029</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1703122999818838</v>
+        <v>0.97297641452823225</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.46367092718527392</v>
+        <v>-1.6891863306103978</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5312969258749813</v>
+        <v>0.7616151363010184</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3674859775959467</v>
+        <v>3.0460122683627002</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.70172213117501592</v>
+        <v>2.7295764589766325</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.4023991672928233</v>
+        <v>5.9178158193134518</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.4866507207201431</v>
+        <v>5.3030144990120753</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.16343010615476317</v>
+        <v>2.1736081553222206</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.9181924652303834</v>
+        <v>-1.36250522309819</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.8408882171742533E-2</v>
+        <v>4.5437306038434482</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2682011677714478</v>
+        <v>3.3416643298567088</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.9472974562490224</v>
+        <v>1.8366844921083914</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.34904158249242112</v>
+        <v>4.1813494037131793</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>3.266817508921295</v>
+        <v>2.1820481840969688</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25954365607038277</v>
+        <v>-1.5868431635874543</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.76128427756078132</v>
+        <v>1.3020601367678912</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1000811026028074</v>
+        <v>-1.1300883618037034</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9105376564883851</v>
+        <v>0.780069446922254</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1962195710270098</v>
+        <v>-0.81214151724536432</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0854499683790513</v>
+        <v>0.45400281419021793</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.473091568882511</v>
+        <v>-1.5880682331540892</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>6.7633867664841496</v>
+        <v>0.76035307419624232</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.1728153010148041</v>
+        <v>1.2173976928406356</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0761156514756909</v>
+        <v>0.89275871457325096</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8162283992485637</v>
+        <v>-2.1602932024693251</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3617205511543009</v>
+        <v>4.5236388974069488</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7371053804915668</v>
+        <v>3.7818159806879521</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.0192470549952475</v>
+        <v>4.2789821412298643</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.71356686802729818</v>
+        <v>2.2542062437996666</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>1.450258747157303</v>
+        <v>6.306163192254477E-2</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7808952575906005</v>
+        <v>0.66240002413797594</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.42856109510529627</v>
+        <v>0.24324202330469769</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7830933567128788</v>
+        <v>-2.3920878756201445</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.25714011174117068</v>
+        <v>0.66506802148368305</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.2632137095731484</v>
+        <v>5.1877801519829809</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.40107288557074838</v>
+        <v>2.621285304395343</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.5134982299152249</v>
+        <v>3.8333481838934675</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93649941854388397</v>
+        <v>3.3984363750746889</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3670728572225492</v>
+        <v>-2.3890705034081581</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81114395694911767</v>
+        <v>2.7480928081947171</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.6370034785709182</v>
+        <v>6.4266623906207023</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.83465845457814591</v>
+        <v>-0.34473787240880771</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2897243910333067</v>
+        <v>2.2698154426710406</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3409671781995014</v>
+        <v>1.2643073111939849</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.9585947972077229</v>
+        <v>0.82700656596336763</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0038038361103503</v>
+        <v>3.9940559680814758</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.2205376122308822</v>
+        <v>4.5174985325126116</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3022047812868136</v>
+        <v>3.2345535092800031</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.95524240906279356</v>
+        <v>4.5187355657756259</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0583706158935602</v>
+        <v>2.4127521765245508</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.2717016201085496E-2</v>
+        <v>2.4574456210990192</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7612978816469411</v>
+        <v>6.007640936758893</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.69685395251094562</v>
+        <v>3.0835992689147602</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5084947949306944</v>
+        <v>5.7121644987271569</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4701371716616958</v>
+        <v>-0.38102901318748561</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.54048570004937879</v>
+        <v>1.6893657165136569</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.98536978404206543</v>
+        <v>4.9478479297333813</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7834804608351735</v>
+        <v>-2.7472055384364955</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6871953111311218</v>
+        <v>-1.1699474711073461</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.96337657582994485</v>
+        <v>-0.81591119237525689</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2894515306346515</v>
+        <v>0.14990756408521255</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5393681805461092</v>
+        <v>4.9867932581025514</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1617795481698474</v>
+        <v>1.7861361219643115</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7229008068354617E-3</v>
+        <v>6.3997084791563896</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9991597346338574</v>
+        <v>5.8179978855963963</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2549138785529257</v>
+        <v>6.010861103991024</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.4390570889391157</v>
+        <v>6.4613444100927495</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.109436690978395</v>
+        <v>1.2504598834629626</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3741687657774007</v>
+        <v>6.893443617138427</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0251684801028116</v>
+        <v>2.2089384784338275</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4612708334788955</v>
+        <v>6.0641249273154934</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.5359178279431367</v>
+        <v>-2.6839834709097627</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2246286223385177</v>
+        <v>-1.9551352228703196</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.7322114657946823E-2</v>
+        <v>-1.4144479885519829</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0651658541582609</v>
+        <v>6.0302544614307543</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8332529748901658</v>
+        <v>2.0785845756642036</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.9224340591288129</v>
+        <v>-1.3021625131223065</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.64495308845509758</v>
+        <v>2.1435956940663861</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.9143513147846152</v>
+        <v>0.37702803279760877</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.7680054279858517</v>
+        <v>1.7824912068195875</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9838241422893077</v>
+        <v>4.1283512241771794</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.44859578382401</v>
+        <v>6.4961313231808315</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.6023856619669392</v>
+        <v>3.1031663552363753E-2</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.35657585818196047</v>
+        <v>-0.12066529961161176</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96408597979283872</v>
+        <v>-2.0630563515512721</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.9769991979152906</v>
+        <v>3.087454144586701</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9398191489824583</v>
+        <v>-2.6217260915621186</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6250018914565274</v>
+        <v>2.3505396256964062</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4002135201705066E-3</v>
+        <v>6.3651638311060275</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.8319262321134451</v>
+        <v>5.6771997975650521</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27344216486341288</v>
+        <v>-1.3914641011794233</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>4.900218264559439</v>
+        <v>-0.96294419472660309</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5157551620877534</v>
+        <v>5.1007552641653238</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.99673381535887184</v>
+        <v>4.0170594345749437</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4373185172766512</v>
+        <v>3.7887512199059614</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>1.309757543942573</v>
+        <v>-2.2763833688339057</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6106641251253784</v>
+        <v>4.0038409254847034</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>1.446889181903857</v>
+        <v>6.9727432226461605</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.4996677434866852</v>
+        <v>-0.15564238009735654</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3146755765392726</v>
+        <v>5.8404113503503083</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6841063251739268</v>
+        <v>5.8447670278717716</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.8910792322805485</v>
+        <v>-1.6430100825285749</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7492799515614301</v>
+        <v>-1.0799363637658461</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71621271807293319</v>
+        <v>5.3789803848314897</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.69665699078526888</v>
+        <v>-1.6061516092986523</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6594139776781827</v>
+        <v>-3.0255804668377184E-2</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7152334270779708</v>
+        <v>2.2084740354851284</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6450963412880375</v>
+        <v>3.4748010377564587</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1002999894587884</v>
+        <v>5.8413444789528466</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7868958623109317</v>
+        <v>1.9528298286323498</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.8086647602023627</v>
+        <v>2.1396815459418743</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.80987443878919407</v>
+        <v>3.2950549620416938</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.75532098489913446</v>
+        <v>6.4402409594023133</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1318548711026999</v>
+        <v>-0.42052811480195995</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0221205129459552</v>
+        <v>6.4198292496392995</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.9380326143316058</v>
+        <v>-0.57658876821743288</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.6773514995914098E-2</v>
+        <v>1.1902793609858424</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.6992939888048402</v>
+        <v>4.6302957182637012</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5706885462778324</v>
+        <v>5.4145971051278199</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7471161504895729</v>
+        <v>-2.140469592384326</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.4505437332341113</v>
+        <v>-1.5509540206006185</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.2836584598516367E-2</v>
+        <v>3.8022148532747249</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.3360452693119598</v>
+        <v>3.9222737306118862</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9576098145688681</v>
+        <v>6.1459378315165925</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>5.2891631805456623</v>
+        <v>-1.7060668564374721</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0474552282226242</v>
+        <v>-2.9602658274143572</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.2032099343413325</v>
+        <v>4.1934235877943316E-2</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>5.8694502247522458</v>
+        <v>-2.7698190123913764</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.0947383473644008</v>
+        <v>0.61116467490598669</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2842866641609305</v>
+        <v>6.2211754044852228</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="1"/>
-        <v>5.6847533585004175</v>
+        <v>1.6872778058184164</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5571453641889628</v>
+        <v>0.91537782744292961</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>1.8126536808966893</v>
+        <v>-2.7092609952710234E-3</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.5849819341402198</v>
+        <v>2.7652051909896231</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.2841927192588183</v>
+        <v>5.3604775475285997</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.56820485015291666</v>
+        <v>4.6738204169037028</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>5.7572117929549496</v>
+        <v>5.71125064013364</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.2305324750765196</v>
+        <v>3.8524339832472556</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.0640527601216094</v>
+        <v>0.8474680289882448</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>6.3315409365564115</v>
+        <v>3.0048596449991329</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="1"/>
-        <v>6.8737537734676053</v>
+        <v>-0.18399490132810348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor of components in QR algorithm
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/BulgeChaserTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/BulgeChaserTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-240" yWindow="1605" windowWidth="19440" windowHeight="11040" activeTab="4"/>
+    <workbookView xWindow="4935" yWindow="195" windowWidth="19440" windowHeight="11010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="By Diag 6x6" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="35">
   <si>
     <t>#1</t>
   </si>
@@ -112,6 +112,18 @@
   </si>
   <si>
     <t>#5</t>
+  </si>
+  <si>
+    <t>Q=</t>
+  </si>
+  <si>
+    <t>#11</t>
+  </si>
+  <si>
+    <t>Verification=</t>
+  </si>
+  <si>
+    <t>Delta=</t>
   </si>
 </sst>
 </file>
@@ -3330,7 +3342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC20"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
@@ -5082,10 +5094,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM53"/>
+  <dimension ref="A1:AT78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5101,12 +5113,12 @@
     <col min="36" max="39" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
@@ -5125,8 +5137,11 @@
       <c r="AH2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-2.4894028533397057</v>
       </c>
@@ -5233,8 +5248,27 @@
       <c r="AM3">
         <v>3.1912023760579356</v>
       </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO3">
+        <f t="array" ref="AO3:AT8">MMULT(TRANSPOSE(M3:R8),TRANSPOSE(T3:Y8))</f>
+        <v>1</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.33746994594368651</v>
       </c>
@@ -5336,8 +5370,26 @@
       <c r="AM4">
         <v>2.7668549840000694</v>
       </c>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>5.3953017766065155E-2</v>
+      </c>
+      <c r="AQ4">
+        <v>-0.9985298653715472</v>
+      </c>
+      <c r="AR4">
+        <v>5.2134283359912079E-3</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6.216734007688931</v>
       </c>
@@ -5430,8 +5482,26 @@
       <c r="AM5">
         <v>-0.59249258111385839</v>
       </c>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>0.99390053661167321</v>
+      </c>
+      <c r="AQ5">
+        <v>5.4204316812223159E-2</v>
+      </c>
+      <c r="AR5">
+        <v>9.6039655153214706E-2</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-0.60160147704533973</v>
       </c>
@@ -5539,8 +5609,26 @@
       <c r="AM6">
         <v>5.405982543789845</v>
       </c>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>-9.6181054251671186E-2</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0.99536385548352979</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -5638,8 +5726,26 @@
       <c r="AM7">
         <v>5.7573222829258839</v>
       </c>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
+        <v>1</v>
+      </c>
+      <c r="AT7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -5730,13 +5836,31 @@
       <c r="AM8">
         <v>5.6781754370638247</v>
       </c>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>0</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -5756,7 +5880,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f>AA3</f>
         <v>-2.4894028533397057</v>
@@ -5869,8 +5993,27 @@
       <c r="AM12">
         <v>3.1912023760579356</v>
       </c>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO12">
+        <f t="array" ref="AO12:AT17">MMULT(MMULT(AO3:AT8,TRANSPOSE(M12:R17)),TRANSPOSE(T12:Y17))</f>
+        <v>1</v>
+      </c>
+      <c r="AP12">
+        <v>0</v>
+      </c>
+      <c r="AQ12">
+        <v>0</v>
+      </c>
+      <c r="AR12">
+        <v>0</v>
+      </c>
+      <c r="AS12">
+        <v>0</v>
+      </c>
+      <c r="AT12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f>AA4</f>
         <v>6.2548854525046629</v>
@@ -5974,8 +6117,26 @@
       <c r="AM13">
         <v>2.7668549840000694</v>
       </c>
-    </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO13">
+        <v>0</v>
+      </c>
+      <c r="AP13">
+        <v>5.3953017766065155E-2</v>
+      </c>
+      <c r="AQ13">
+        <v>0.68511374647685352</v>
+      </c>
+      <c r="AR13">
+        <v>0.72640298716715468</v>
+      </c>
+      <c r="AS13">
+        <v>6.8502917469874377E-3</v>
+      </c>
+      <c r="AT13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ref="A14:F17" si="1">AH5</f>
         <v>0</v>
@@ -6076,8 +6237,26 @@
       <c r="AM14">
         <v>4.2984630141770257</v>
       </c>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO14">
+        <v>0</v>
+      </c>
+      <c r="AP14">
+        <v>0.99390053661167321</v>
+      </c>
+      <c r="AQ14">
+        <v>3.322092279932639E-2</v>
+      </c>
+      <c r="AR14">
+        <v>-0.10515694592209993</v>
+      </c>
+      <c r="AS14">
+        <v>3.3216821943773527E-4</v>
+      </c>
+      <c r="AT14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -6190,8 +6369,26 @@
       <c r="AM15">
         <v>-3.2555848906756695</v>
       </c>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO15">
+        <v>0</v>
+      </c>
+      <c r="AP15">
+        <v>-9.6181054251671186E-2</v>
+      </c>
+      <c r="AQ15">
+        <v>0.72760948272939763</v>
+      </c>
+      <c r="AR15">
+        <v>-0.67917649912152511</v>
+      </c>
+      <c r="AS15">
+        <v>7.2751966519465925E-3</v>
+      </c>
+      <c r="AT15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -6297,8 +6494,26 @@
       <c r="AM16">
         <v>5.8005893948172922</v>
       </c>
-    </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO16">
+        <v>0</v>
+      </c>
+      <c r="AP16">
+        <v>0</v>
+      </c>
+      <c r="AQ16">
+        <v>-9.9982658030952319E-3</v>
+      </c>
+      <c r="AR16">
+        <v>0</v>
+      </c>
+      <c r="AS16">
+        <v>0.99995001609126977</v>
+      </c>
+      <c r="AT16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -6395,13 +6610,31 @@
       <c r="AM17">
         <v>5.6781754370638247</v>
       </c>
-    </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO17">
+        <v>0</v>
+      </c>
+      <c r="AP17">
+        <v>0</v>
+      </c>
+      <c r="AQ17">
+        <v>0</v>
+      </c>
+      <c r="AR17">
+        <v>0</v>
+      </c>
+      <c r="AS17">
+        <v>0</v>
+      </c>
+      <c r="AT17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
@@ -6421,7 +6654,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f>A12</f>
         <v>-2.4894028533397057</v>
@@ -6534,8 +6767,27 @@
       <c r="AM21">
         <v>3.1880534252876012</v>
       </c>
-    </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO21">
+        <f t="array" ref="AO21:AT26">MMULT(MMULT(AO12:AT17,TRANSPOSE(M21:R26)),TRANSPOSE(T21:Y26))</f>
+        <v>1</v>
+      </c>
+      <c r="AP21">
+        <v>0</v>
+      </c>
+      <c r="AQ21">
+        <v>0</v>
+      </c>
+      <c r="AR21">
+        <v>0</v>
+      </c>
+      <c r="AS21">
+        <v>0</v>
+      </c>
+      <c r="AT21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f>A13</f>
         <v>6.2548854525046629</v>
@@ -6639,8 +6891,26 @@
       <c r="AM22">
         <v>2.7629351379914122</v>
       </c>
-    </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO22">
+        <v>0</v>
+      </c>
+      <c r="AP22">
+        <v>5.3953017766065155E-2</v>
+      </c>
+      <c r="AQ22">
+        <v>0.68511374647685352</v>
+      </c>
+      <c r="AR22">
+        <v>0.71401929649406792</v>
+      </c>
+      <c r="AS22">
+        <v>-0.13373122989075714</v>
+      </c>
+      <c r="AT22">
+        <v>7.9287351207769658E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f>AA14</f>
         <v>0</v>
@@ -6737,8 +7007,26 @@
       <c r="AM23">
         <v>4.2995970603591545</v>
       </c>
-    </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO23">
+        <v>0</v>
+      </c>
+      <c r="AP23">
+        <v>0.99390053661167321</v>
+      </c>
+      <c r="AQ23">
+        <v>3.322092279932639E-2</v>
+      </c>
+      <c r="AR23">
+        <v>-0.1031082652619331</v>
+      </c>
+      <c r="AS23">
+        <v>2.065831883052853E-2</v>
+      </c>
+      <c r="AT23">
+        <v>-1.1449524236092806E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ref="A24:F26" si="4">AH15</f>
         <v>0</v>
@@ -6853,8 +7141,26 @@
       <c r="AM24">
         <v>-2.0738849714122982</v>
       </c>
-    </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO24">
+        <v>0</v>
+      </c>
+      <c r="AP24">
+        <v>-9.6181054251671186E-2</v>
+      </c>
+      <c r="AQ24">
+        <v>0.72760948272939763</v>
+      </c>
+      <c r="AR24">
+        <v>-0.66495283173468644</v>
+      </c>
+      <c r="AS24">
+        <v>0.13845877291111294</v>
+      </c>
+      <c r="AT24">
+        <v>-7.3838828957736803E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -6960,8 +7266,26 @@
       <c r="AM25">
         <v>6.3188301484246479</v>
       </c>
-    </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO25">
+        <v>0</v>
+      </c>
+      <c r="AP25">
+        <v>0</v>
+      </c>
+      <c r="AQ25">
+        <v>-9.9982658030952319E-3</v>
+      </c>
+      <c r="AR25">
+        <v>0.1933432914993316</v>
+      </c>
+      <c r="AS25">
+        <v>0.98108020070682833</v>
+      </c>
+      <c r="AT25">
+        <v>2.1469556259956133E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -7060,13 +7384,31 @@
       <c r="AM26">
         <v>5.6759612236511314</v>
       </c>
-    </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO26">
+        <v>0</v>
+      </c>
+      <c r="AP26">
+        <v>0</v>
+      </c>
+      <c r="AQ26">
+        <v>0</v>
+      </c>
+      <c r="AR26">
+        <v>-1.1104364085631568E-3</v>
+      </c>
+      <c r="AS26">
+        <v>0</v>
+      </c>
+      <c r="AT26">
+        <v>0.99999938346530126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6</v>
       </c>
@@ -7083,7 +7425,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f>A21</f>
         <v>-2.4894028533397057</v>
@@ -7140,6 +7482,24 @@
       <c r="R30">
         <v>0</v>
       </c>
+      <c r="T30">
+        <v>1</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <v>0</v>
+      </c>
       <c r="AA30">
         <f t="array" ref="AA30:AF35">MMULT(M30:R35,AH21:AM26)</f>
         <v>-2.4894028533397057</v>
@@ -7178,8 +7538,27 @@
       <c r="AM30">
         <v>-3.1126403311000792</v>
       </c>
-    </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO30">
+        <f t="array" ref="AO30:AT35">MMULT(MMULT(AO21:AT26,TRANSPOSE(M30:R35)),TRANSPOSE(T30:Y35))</f>
+        <v>1</v>
+      </c>
+      <c r="AP30">
+        <v>0</v>
+      </c>
+      <c r="AQ30">
+        <v>0</v>
+      </c>
+      <c r="AR30">
+        <v>0</v>
+      </c>
+      <c r="AS30">
+        <v>0</v>
+      </c>
+      <c r="AT30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" ref="A31:F32" si="6">A22</f>
         <v>6.2548854525046629</v>
@@ -7229,6 +7608,24 @@
       <c r="R31">
         <v>0</v>
       </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <v>0</v>
+      </c>
       <c r="AA31">
         <v>6.2548854525046629</v>
       </c>
@@ -7265,8 +7662,26 @@
       <c r="AM31">
         <v>-2.7568774770130799</v>
       </c>
-    </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO31">
+        <v>0</v>
+      </c>
+      <c r="AP31">
+        <v>5.3953017766065155E-2</v>
+      </c>
+      <c r="AQ31">
+        <v>0.68511374647685352</v>
+      </c>
+      <c r="AR31">
+        <v>0.71401929649406792</v>
+      </c>
+      <c r="AS31">
+        <v>0.13360947068717108</v>
+      </c>
+      <c r="AT31">
+        <v>5.7601943712573354E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -7309,6 +7724,24 @@
       <c r="R32">
         <v>0</v>
       </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>1</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <v>0</v>
+      </c>
       <c r="AA32">
         <v>0</v>
       </c>
@@ -7345,8 +7778,26 @@
       <c r="AM32">
         <v>-4.2636638408315832</v>
       </c>
-    </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO32">
+        <v>0</v>
+      </c>
+      <c r="AP32">
+        <v>0.99390053661167321</v>
+      </c>
+      <c r="AQ32">
+        <v>3.322092279932639E-2</v>
+      </c>
+      <c r="AR32">
+        <v>-0.1031082652619331</v>
+      </c>
+      <c r="AS32">
+        <v>-2.0639118684747632E-2</v>
+      </c>
+      <c r="AT32">
+        <v>-8.9778949715072724E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f>AA24</f>
         <v>0</v>
@@ -7389,6 +7840,24 @@
       <c r="R33">
         <v>0</v>
       </c>
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>1</v>
+      </c>
+      <c r="X33">
+        <v>0</v>
+      </c>
+      <c r="Y33">
+        <v>0</v>
+      </c>
       <c r="AA33">
         <v>0</v>
       </c>
@@ -7425,8 +7894,26 @@
       <c r="AM33">
         <v>2.0047682841310057</v>
       </c>
-    </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO33">
+        <v>0</v>
+      </c>
+      <c r="AP33">
+        <v>-9.6181054251671186E-2</v>
+      </c>
+      <c r="AQ33">
+        <v>0.72760948272939763</v>
+      </c>
+      <c r="AR33">
+        <v>-0.66495283173468644</v>
+      </c>
+      <c r="AS33">
+        <v>-0.13832866663584117</v>
+      </c>
+      <c r="AT33">
+        <v>-6.0462385056867067E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" ref="A34:F35" si="8">AH25</f>
         <v>0</v>
@@ -7471,6 +7958,24 @@
         <f>K31</f>
         <v>4.899465651995584E-2</v>
       </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <v>0</v>
+      </c>
+      <c r="X34">
+        <v>1</v>
+      </c>
+      <c r="Y34">
+        <v>0</v>
+      </c>
       <c r="AA34">
         <v>0</v>
       </c>
@@ -7507,8 +8012,26 @@
       <c r="AM34">
         <v>5.9994768666229783</v>
       </c>
-    </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO34">
+        <v>0</v>
+      </c>
+      <c r="AP34">
+        <v>0</v>
+      </c>
+      <c r="AQ34">
+        <v>-9.9982658030952319E-3</v>
+      </c>
+      <c r="AR34">
+        <v>0.1933432914993316</v>
+      </c>
+      <c r="AS34">
+        <v>-0.9798914443456509</v>
+      </c>
+      <c r="AT34">
+        <v>-4.8282125174119776E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -7553,6 +8076,24 @@
         <f>Q34</f>
         <v>-0.99879904066458314</v>
       </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <v>0</v>
+      </c>
+      <c r="X35">
+        <v>0</v>
+      </c>
+      <c r="Y35">
+        <v>1</v>
+      </c>
       <c r="AA35">
         <v>0</v>
       </c>
@@ -7589,13 +8130,31 @@
       <c r="AM35">
         <v>5.9902149635780759</v>
       </c>
-    </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO35">
+        <v>0</v>
+      </c>
+      <c r="AP35">
+        <v>0</v>
+      </c>
+      <c r="AQ35">
+        <v>0</v>
+      </c>
+      <c r="AR35">
+        <v>-1.1104364085631568E-3</v>
+      </c>
+      <c r="AS35">
+        <v>4.8994626313050044E-2</v>
+      </c>
+      <c r="AT35">
+        <v>-0.99879842487031745</v>
+      </c>
+    </row>
+    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>6</v>
       </c>
@@ -7603,7 +8162,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f>A30</f>
         <v>-2.4894028533397057</v>
@@ -7629,7 +8188,7 @@
         <v>3.1912023760579356</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" ref="A40:F42" si="10">A31</f>
         <v>6.2548854525046629</v>
@@ -7655,7 +8214,7 @@
         <v>2.7668549840000694</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -7681,7 +8240,7 @@
         <v>4.2984630141770257</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -7707,7 +8266,7 @@
         <v>-2.0788917112384273</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f>AA34</f>
         <v>0</v>
@@ -7733,7 +8292,7 @@
         <v>-6.0331497197956079</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" ref="A44:F44" si="12">AH35</f>
         <v>0</v>
@@ -7759,12 +8318,12 @@
         <v>5.9902149635780759</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>6</v>
       </c>
@@ -7772,7 +8331,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A48">
         <f>AH30</f>
         <v>-2.4894028533397057</v>
@@ -7926,6 +8485,462 @@
       <c r="F53">
         <f t="shared" si="19"/>
         <v>5.9902149635780759</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>6</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f>AO30</f>
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <f t="shared" ref="B57:F62" si="20">AP30</f>
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" ref="A58:A62" si="21">AO31</f>
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="20"/>
+        <v>5.3953017766065155E-2</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="20"/>
+        <v>0.68511374647685352</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="20"/>
+        <v>0.71401929649406792</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="20"/>
+        <v>0.13360947068717108</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="20"/>
+        <v>5.7601943712573354E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="20"/>
+        <v>0.99390053661167321</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="20"/>
+        <v>3.322092279932639E-2</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="20"/>
+        <v>-0.1031082652619331</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="20"/>
+        <v>-2.0639118684747632E-2</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="20"/>
+        <v>-8.9778949715072724E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="20"/>
+        <v>-9.6181054251671186E-2</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="20"/>
+        <v>0.72760948272939763</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="20"/>
+        <v>-0.66495283173468644</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="20"/>
+        <v>-0.13832866663584117</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="20"/>
+        <v>-6.0462385056867067E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="20"/>
+        <v>-9.9982658030952319E-3</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="20"/>
+        <v>0.1933432914993316</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="20"/>
+        <v>-0.9798914443456509</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="20"/>
+        <v>-4.8282125174119776E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="20"/>
+        <v>-1.1104364085631568E-3</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="20"/>
+        <v>4.8994626313050044E-2</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="20"/>
+        <v>-0.99879842487031745</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="array" ref="A65:F70">MMULT(MMULT(A57:F62,A48:F53),TRANSPOSE(A57:F62))</f>
+        <v>-2.4894028533397057</v>
+      </c>
+      <c r="B65">
+        <v>-1.2208340311620398</v>
+      </c>
+      <c r="C65">
+        <v>5.4870796290101262</v>
+      </c>
+      <c r="D65">
+        <v>1.5227302569475187</v>
+      </c>
+      <c r="E65">
+        <v>-1.9860942179327741</v>
+      </c>
+      <c r="F65">
+        <v>3.191202376057936</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>0.33746994594368657</v>
+      </c>
+      <c r="B66">
+        <v>6.153136668723481</v>
+      </c>
+      <c r="C66">
+        <v>6.1565699511311651</v>
+      </c>
+      <c r="D66">
+        <v>0.10492755903255384</v>
+      </c>
+      <c r="E66">
+        <v>1.3135676263083487</v>
+      </c>
+      <c r="F66">
+        <v>0.76908541593881163</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>6.2167340076889328</v>
+      </c>
+      <c r="B67">
+        <v>-2.128868559198843</v>
+      </c>
+      <c r="C67">
+        <v>4.2939391756076954</v>
+      </c>
+      <c r="D67">
+        <v>2.7295065982736268</v>
+      </c>
+      <c r="E67">
+        <v>-0.99764117327967083</v>
+      </c>
+      <c r="F67">
+        <v>3.2370516970186398</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>-0.60160147704533984</v>
+      </c>
+      <c r="B68">
+        <v>-1.46242203146758</v>
+      </c>
+      <c r="C68">
+        <v>6.4158939135670217</v>
+      </c>
+      <c r="D68">
+        <v>0.11882881748661028</v>
+      </c>
+      <c r="E68">
+        <v>-1.8068818306006229</v>
+      </c>
+      <c r="F68">
+        <v>5.114800598140703</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>0</v>
+      </c>
+      <c r="B69">
+        <v>1.5265566588595902E-16</v>
+      </c>
+      <c r="C69">
+        <v>1.1275702593849246E-17</v>
+      </c>
+      <c r="D69">
+        <v>0.94773247089143309</v>
+      </c>
+      <c r="E69">
+        <v>-0.37935419014503241</v>
+      </c>
+      <c r="F69">
+        <v>5.7573222829258839</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>0</v>
+      </c>
+      <c r="B70">
+        <v>1.3877787807814457E-17</v>
+      </c>
+      <c r="C70">
+        <v>-1.7347234759768071E-18</v>
+      </c>
+      <c r="D70">
+        <v>-2.0816681711721685E-17</v>
+      </c>
+      <c r="E70">
+        <v>0.41316797981082509</v>
+      </c>
+      <c r="F70">
+        <v>5.6781754370638255</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f>A65-A3</f>
+        <v>0</v>
+      </c>
+      <c r="B73">
+        <f t="shared" ref="B73:F73" si="22">B65-B3</f>
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" ref="A74:F78" si="23">A66-A4</f>
+        <v>0</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="23"/>
+        <v>-6.2450045135165055E-16</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="23"/>
+        <v>-2.7755575615628914E-16</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="23"/>
+        <v>1.5265566588595902E-16</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="23"/>
+        <v>1.1275702593849246E-17</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="23"/>
+        <v>1.3877787807814457E-17</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="23"/>
+        <v>-1.7347234759768071E-18</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="23"/>
+        <v>-2.0816681711721685E-17</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="23"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7935,10 +8950,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM53"/>
+  <dimension ref="A1:AT78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7952,14 +8967,17 @@
     <col min="30" max="32" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="34" max="35" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="36" max="39" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="44" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
@@ -7978,8 +8996,11 @@
       <c r="AH2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4.1299190577623675</v>
       </c>
@@ -8086,8 +9107,27 @@
       <c r="AM3">
         <v>-1.3341115715941216</v>
       </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO3">
+        <f t="array" ref="AO3:AT8">MMULT(TRANSPOSE(M3:R8),TRANSPOSE(T3:Y8))</f>
+        <v>1</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2.6557026101959611</v>
       </c>
@@ -8189,8 +9229,26 @@
       <c r="AM4">
         <v>-1.567462886617184</v>
       </c>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0.56080361895784447</v>
+      </c>
+      <c r="AQ4">
+        <v>0.25238811331010003</v>
+      </c>
+      <c r="AR4">
+        <v>-0.78854266924723404</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-0.69269295415944798</v>
       </c>
@@ -8283,8 +9341,26 @@
       <c r="AM5">
         <v>0.52018515223979545</v>
       </c>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>-0.14627568389163664</v>
+      </c>
+      <c r="AQ5">
+        <v>0.96762608494178581</v>
+      </c>
+      <c r="AR5">
+        <v>0.20567737853800519</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3.8591020581643383</v>
       </c>
@@ -8392,8 +9468,26 @@
       <c r="AM6">
         <v>-0.2460210334865871</v>
       </c>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0.81492498137302105</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0.57956645411391883</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -8492,8 +9586,26 @@
       <c r="AM7">
         <v>3.4960354799137559</v>
       </c>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
+        <v>1</v>
+      </c>
+      <c r="AT7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -8584,13 +9696,31 @@
       <c r="AM8">
         <v>3.4350466320112147</v>
       </c>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>0</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -8610,7 +9740,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f>AA3</f>
         <v>4.1299190577623675</v>
@@ -8723,8 +9853,27 @@
       <c r="AM12">
         <v>-1.3341115715941216</v>
       </c>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO12">
+        <f t="array" ref="AO12:AT17">MMULT(MMULT(AO3:AT8,TRANSPOSE(M12:R17)),TRANSPOSE(T12:Y17))</f>
+        <v>1</v>
+      </c>
+      <c r="AP12">
+        <v>0</v>
+      </c>
+      <c r="AQ12">
+        <v>0</v>
+      </c>
+      <c r="AR12">
+        <v>0</v>
+      </c>
+      <c r="AS12">
+        <v>0</v>
+      </c>
+      <c r="AT12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f>AA4</f>
         <v>4.7355304431364402</v>
@@ -8828,8 +9977,26 @@
       <c r="AM13">
         <v>-1.567462886617184</v>
       </c>
-    </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO13">
+        <v>0</v>
+      </c>
+      <c r="AP13">
+        <v>0.56080361895784447</v>
+      </c>
+      <c r="AQ13">
+        <v>0.58021193490052836</v>
+      </c>
+      <c r="AR13">
+        <v>-0.59063813927206699</v>
+      </c>
+      <c r="AS13">
+        <v>-1.2049102590707679E-16</v>
+      </c>
+      <c r="AT13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ref="A14:F17" si="1">AH5</f>
         <v>1.1102230246251565E-16</v>
@@ -8930,8 +10097,26 @@
       <c r="AM14">
         <v>0.57525019652877096</v>
       </c>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO14">
+        <v>0</v>
+      </c>
+      <c r="AP14">
+        <v>-0.14627568389163664</v>
+      </c>
+      <c r="AQ14">
+        <v>0.77158602555497668</v>
+      </c>
+      <c r="AR14">
+        <v>0.61907869408525817</v>
+      </c>
+      <c r="AS14">
+        <v>-1.6023315999285981E-16</v>
+      </c>
+      <c r="AT14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>-4.4408920985006262E-16</v>
@@ -9044,8 +10229,26 @@
       <c r="AM15">
         <v>1.4358026401940449E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO15">
+        <v>0</v>
+      </c>
+      <c r="AP15">
+        <v>0.81492498137302105</v>
+      </c>
+      <c r="AQ15">
+        <v>-0.26078557430820376</v>
+      </c>
+      <c r="AR15">
+        <v>0.51757913304819536</v>
+      </c>
+      <c r="AS15">
+        <v>5.4156627087563666E-17</v>
+      </c>
+      <c r="AT15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9151,8 +10354,26 @@
       <c r="AM16">
         <v>3.4960354799137559</v>
       </c>
-    </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO16">
+        <v>0</v>
+      </c>
+      <c r="AP16">
+        <v>0</v>
+      </c>
+      <c r="AQ16">
+        <v>2.0766726545832568E-16</v>
+      </c>
+      <c r="AR16">
+        <v>0</v>
+      </c>
+      <c r="AS16">
+        <v>1</v>
+      </c>
+      <c r="AT16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9249,13 +10470,31 @@
       <c r="AM17">
         <v>3.4350466320112147</v>
       </c>
-    </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO17">
+        <v>0</v>
+      </c>
+      <c r="AP17">
+        <v>0</v>
+      </c>
+      <c r="AQ17">
+        <v>0</v>
+      </c>
+      <c r="AR17">
+        <v>0</v>
+      </c>
+      <c r="AS17">
+        <v>0</v>
+      </c>
+      <c r="AT17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
@@ -9275,7 +10514,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f>A12</f>
         <v>4.1299190577623675</v>
@@ -9388,8 +10627,27 @@
       <c r="AM21">
         <v>-1.3341115715941219</v>
       </c>
-    </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO21">
+        <f t="array" ref="AO21:AT26">MMULT(MMULT(AO12:AT17,TRANSPOSE(M21:R26)),TRANSPOSE(T21:Y26))</f>
+        <v>1</v>
+      </c>
+      <c r="AP21">
+        <v>0</v>
+      </c>
+      <c r="AQ21">
+        <v>0</v>
+      </c>
+      <c r="AR21">
+        <v>0</v>
+      </c>
+      <c r="AS21">
+        <v>0</v>
+      </c>
+      <c r="AT21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f>A13</f>
         <v>4.7355304431364402</v>
@@ -9493,8 +10751,26 @@
       <c r="AM22">
         <v>-1.5674628866171845</v>
       </c>
-    </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO22">
+        <v>0</v>
+      </c>
+      <c r="AP22">
+        <v>0.56080361895784447</v>
+      </c>
+      <c r="AQ22">
+        <v>0.58021193490052836</v>
+      </c>
+      <c r="AR22">
+        <v>-0.59063813927206699</v>
+      </c>
+      <c r="AS22">
+        <v>-1.3749155639743616E-16</v>
+      </c>
+      <c r="AT22">
+        <v>1.1902039138080138E-16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f>AA14</f>
         <v>2.9897328505201868E-16</v>
@@ -9591,8 +10867,26 @@
       <c r="AM23">
         <v>0.57525019652877152</v>
       </c>
-    </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO23">
+        <v>0</v>
+      </c>
+      <c r="AP23">
+        <v>-0.14627568389163664</v>
+      </c>
+      <c r="AQ23">
+        <v>0.77158602555497668</v>
+      </c>
+      <c r="AR23">
+        <v>0.61907869408525817</v>
+      </c>
+      <c r="AS23">
+        <v>-1.424140157234101E-16</v>
+      </c>
+      <c r="AT23">
+        <v>-1.2475149091515419E-16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ref="A24:F26" si="4">AH15</f>
         <v>-3.4663547535492615E-16</v>
@@ -9707,8 +11001,26 @@
       <c r="AM24">
         <v>1.4358026401940786E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO24">
+        <v>0</v>
+      </c>
+      <c r="AP24">
+        <v>0.81492498137302105</v>
+      </c>
+      <c r="AQ24">
+        <v>-0.26078557430820376</v>
+      </c>
+      <c r="AR24">
+        <v>0.51757913304819536</v>
+      </c>
+      <c r="AS24">
+        <v>6.9054276337583481E-17</v>
+      </c>
+      <c r="AT24">
+        <v>-1.0429815971900182E-16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="4"/>
         <v>-6.2086964551845232E-32</v>
@@ -9814,8 +11126,26 @@
       <c r="AM25">
         <v>3.4960354799137559</v>
       </c>
-    </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO25">
+        <v>0</v>
+      </c>
+      <c r="AP25">
+        <v>0</v>
+      </c>
+      <c r="AQ25">
+        <v>2.0766726545832568E-16</v>
+      </c>
+      <c r="AR25">
+        <v>-2.8783326642792994E-17</v>
+      </c>
+      <c r="AS25">
+        <v>1</v>
+      </c>
+      <c r="AT25">
+        <v>5.8001720080061314E-33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -9914,13 +11244,31 @@
       <c r="AM26">
         <v>3.4350466320112147</v>
       </c>
-    </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO26">
+        <v>0</v>
+      </c>
+      <c r="AP26">
+        <v>0</v>
+      </c>
+      <c r="AQ26">
+        <v>0</v>
+      </c>
+      <c r="AR26">
+        <v>2.015115236674155E-16</v>
+      </c>
+      <c r="AS26">
+        <v>0</v>
+      </c>
+      <c r="AT26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6</v>
       </c>
@@ -9937,7 +11285,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f>A21</f>
         <v>4.1299190577623675</v>
@@ -9994,6 +11342,24 @@
       <c r="R30">
         <v>0</v>
       </c>
+      <c r="T30">
+        <v>1</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <v>0</v>
+      </c>
       <c r="AA30">
         <f t="array" ref="AA30:AF35">MMULT(M30:R35,AH21:AM26)</f>
         <v>4.1299190577623675</v>
@@ -10032,8 +11398,27 @@
       <c r="AM30">
         <v>-1.9970510277728182</v>
       </c>
-    </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO30">
+        <f t="array" ref="AO30:AT35">MMULT(MMULT(AO21:AT26,TRANSPOSE(M30:R35)),TRANSPOSE(T30:Y35))</f>
+        <v>1</v>
+      </c>
+      <c r="AP30">
+        <v>0</v>
+      </c>
+      <c r="AQ30">
+        <v>0</v>
+      </c>
+      <c r="AR30">
+        <v>0</v>
+      </c>
+      <c r="AS30">
+        <v>0</v>
+      </c>
+      <c r="AT30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" ref="A31:F32" si="6">A22</f>
         <v>4.7355304431364402</v>
@@ -10083,6 +11468,24 @@
       <c r="R31">
         <v>0</v>
       </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <v>0</v>
+      </c>
       <c r="AA31">
         <v>4.7355304431364402</v>
       </c>
@@ -10119,8 +11522,26 @@
       <c r="AM31">
         <v>-1.6420042810570272</v>
       </c>
-    </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO31">
+        <v>0</v>
+      </c>
+      <c r="AP31">
+        <v>0.56080361895784447</v>
+      </c>
+      <c r="AQ31">
+        <v>0.58021193490052836</v>
+      </c>
+      <c r="AR31">
+        <v>-0.59063813927206699</v>
+      </c>
+      <c r="AS31">
+        <v>-1.1469487907778071E-16</v>
+      </c>
+      <c r="AT31">
+        <v>1.4112004236947271E-16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="6"/>
         <v>2.9897328505201868E-16</v>
@@ -10163,6 +11584,24 @@
       <c r="R32">
         <v>0</v>
       </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>1</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <v>0</v>
+      </c>
       <c r="AA32">
         <v>2.9897328505201868E-16</v>
       </c>
@@ -10199,8 +11638,26 @@
       <c r="AM32">
         <v>0.61873298196929627</v>
       </c>
-    </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO32">
+        <v>0</v>
+      </c>
+      <c r="AP32">
+        <v>-0.14627568389163664</v>
+      </c>
+      <c r="AQ32">
+        <v>0.77158602555497668</v>
+      </c>
+      <c r="AR32">
+        <v>0.61907869408525817</v>
+      </c>
+      <c r="AS32">
+        <v>-1.6194124349231111E-16</v>
+      </c>
+      <c r="AT32">
+        <v>-9.8080171371105891E-17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f>AA24</f>
         <v>-3.4663547535492615E-16</v>
@@ -10243,6 +11700,24 @@
       <c r="R33">
         <v>0</v>
       </c>
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>1</v>
+      </c>
+      <c r="X33">
+        <v>0</v>
+      </c>
+      <c r="Y33">
+        <v>0</v>
+      </c>
       <c r="AA33">
         <v>-3.4663547535492615E-16</v>
       </c>
@@ -10279,8 +11754,26 @@
       <c r="AM33">
         <v>0.16908945794825522</v>
       </c>
-    </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO33">
+        <v>0</v>
+      </c>
+      <c r="AP33">
+        <v>0.81492498137302105</v>
+      </c>
+      <c r="AQ33">
+        <v>-0.26078557430820376</v>
+      </c>
+      <c r="AR33">
+        <v>0.51757913304819536</v>
+      </c>
+      <c r="AS33">
+        <v>4.9861322268205931E-17</v>
+      </c>
+      <c r="AT33">
+        <v>-1.1471899469113155E-16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" ref="A34:F35" si="8">AH25</f>
         <v>-7.2064286664965889E-32</v>
@@ -10325,6 +11818,24 @@
         <f>K31</f>
         <v>0.17392872226310796</v>
       </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <v>0</v>
+      </c>
+      <c r="X34">
+        <v>1</v>
+      </c>
+      <c r="Y34">
+        <v>0</v>
+      </c>
       <c r="AA34">
         <v>-5.8816797785376744E-32</v>
       </c>
@@ -10361,8 +11872,26 @@
       <c r="AM34">
         <v>3.5776822072013292</v>
       </c>
-    </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO34">
+        <v>0</v>
+      </c>
+      <c r="AP34">
+        <v>0</v>
+      </c>
+      <c r="AQ34">
+        <v>2.0766726545832568E-16</v>
+      </c>
+      <c r="AR34">
+        <v>-2.8783326642792994E-17</v>
+      </c>
+      <c r="AS34">
+        <v>0.98475824422643077</v>
+      </c>
+      <c r="AT34">
+        <v>-0.17392872226310796</v>
+      </c>
+    </row>
+    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="8"/>
         <v>6.9851042795950027E-32</v>
@@ -10407,6 +11936,24 @@
         <f>Q34</f>
         <v>0.98475824422643077</v>
       </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <v>0</v>
+      </c>
+      <c r="X35">
+        <v>0</v>
+      </c>
+      <c r="Y35">
+        <v>1</v>
+      </c>
       <c r="AA35">
         <v>8.1320439561564882E-32</v>
       </c>
@@ -10443,13 +11990,31 @@
       <c r="AM35">
         <v>2.0558989401770478</v>
       </c>
-    </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AO35">
+        <v>0</v>
+      </c>
+      <c r="AP35">
+        <v>0</v>
+      </c>
+      <c r="AQ35">
+        <v>0</v>
+      </c>
+      <c r="AR35">
+        <v>2.015115236674155E-16</v>
+      </c>
+      <c r="AS35">
+        <v>0.17392872226310796</v>
+      </c>
+      <c r="AT35">
+        <v>0.98475824422643077</v>
+      </c>
+    </row>
+    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>6</v>
       </c>
@@ -10457,7 +12022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f>A30</f>
         <v>4.1299190577623675</v>
@@ -10483,7 +12048,7 @@
         <v>-1.3341115715941216</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" ref="A40:F42" si="10">A31</f>
         <v>4.7355304431364402</v>
@@ -10509,7 +12074,7 @@
         <v>-1.567462886617184</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="10"/>
         <v>2.9897328505201868E-16</v>
@@ -10535,7 +12100,7 @@
         <v>0.57525019652877096</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="10"/>
         <v>-3.4663547535492615E-16</v>
@@ -10561,7 +12126,7 @@
         <v>1.4358026401941041E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f>AA34</f>
         <v>-5.8816797785376744E-32</v>
@@ -10587,7 +12152,7 @@
         <v>4.0402030325730802</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" ref="A44:F44" si="12">AH35</f>
         <v>8.1320439561564882E-32</v>
@@ -10613,12 +12178,12 @@
         <v>2.0558989401770478</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>6</v>
       </c>
@@ -10626,7 +12191,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A48">
         <f>AH30</f>
         <v>4.1299190577623675</v>
@@ -10780,6 +12345,462 @@
       <c r="F53">
         <f t="shared" si="13"/>
         <v>2.0558989401770478</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>6</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f>AO30</f>
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <f t="shared" ref="B57:F57" si="15">AP30</f>
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" ref="A58:A62" si="16">AO31</f>
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <f t="shared" ref="B58:B62" si="17">AP31</f>
+        <v>0.56080361895784447</v>
+      </c>
+      <c r="C58">
+        <f t="shared" ref="C58:C62" si="18">AQ31</f>
+        <v>0.58021193490052836</v>
+      </c>
+      <c r="D58">
+        <f t="shared" ref="D58:D62" si="19">AR31</f>
+        <v>-0.59063813927206699</v>
+      </c>
+      <c r="E58">
+        <f t="shared" ref="E58:E62" si="20">AS31</f>
+        <v>-1.1469487907778071E-16</v>
+      </c>
+      <c r="F58">
+        <f t="shared" ref="F58:F62" si="21">AT31</f>
+        <v>1.4112004236947271E-16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="17"/>
+        <v>-0.14627568389163664</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="18"/>
+        <v>0.77158602555497668</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="19"/>
+        <v>0.61907869408525817</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="20"/>
+        <v>-1.6194124349231111E-16</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="21"/>
+        <v>-9.8080171371105891E-17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="17"/>
+        <v>0.81492498137302105</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="18"/>
+        <v>-0.26078557430820376</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="19"/>
+        <v>0.51757913304819536</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="20"/>
+        <v>4.9861322268205931E-17</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="21"/>
+        <v>-1.1471899469113155E-16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="18"/>
+        <v>2.0766726545832568E-16</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="19"/>
+        <v>-2.8783326642792994E-17</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="20"/>
+        <v>0.98475824422643077</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="21"/>
+        <v>-0.17392872226310796</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="19"/>
+        <v>2.015115236674155E-16</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="20"/>
+        <v>0.17392872226310796</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="21"/>
+        <v>0.98475824422643077</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="array" ref="A65:F70">MMULT(MMULT(A57:F62,A48:F53),TRANSPOSE(A57:F62))</f>
+        <v>4.1299190577623675</v>
+      </c>
+      <c r="B65">
+        <v>2.7864701917357149</v>
+      </c>
+      <c r="C65">
+        <v>2.0306046292172621</v>
+      </c>
+      <c r="D65">
+        <v>3.3256295562164375</v>
+      </c>
+      <c r="E65">
+        <v>3.9284693754836835</v>
+      </c>
+      <c r="F65">
+        <v>-1.3341115715941214</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>2.6557026101959607</v>
+      </c>
+      <c r="B66">
+        <v>-0.11968845256554334</v>
+      </c>
+      <c r="C66">
+        <v>-1.8039115602771592</v>
+      </c>
+      <c r="D66">
+        <v>0.30173185395631047</v>
+      </c>
+      <c r="E66">
+        <v>0.66926435268965834</v>
+      </c>
+      <c r="F66">
+        <v>-0.55375222781482059</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>-0.69269295415944787</v>
+      </c>
+      <c r="B67">
+        <v>4.8981743369651536</v>
+      </c>
+      <c r="C67">
+        <v>0.96551991318403285</v>
+      </c>
+      <c r="D67">
+        <v>1.1051202838375684</v>
+      </c>
+      <c r="E67">
+        <v>-0.8661048000567767</v>
+      </c>
+      <c r="F67">
+        <v>0.68202546678859555</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>3.8591020581643378</v>
+      </c>
+      <c r="B68">
+        <v>-2.5524292049923316</v>
+      </c>
+      <c r="C68">
+        <v>4.8008323897154952</v>
+      </c>
+      <c r="D68">
+        <v>-1.9082676681357242</v>
+      </c>
+      <c r="E68">
+        <v>7.8435013270618109E-2</v>
+      </c>
+      <c r="F68">
+        <v>-1.4199502016946732</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>-1.3684555315672042E-47</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>-9.8607613152626476E-32</v>
+      </c>
+      <c r="D69">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="E69">
+        <v>1.593627460433078</v>
+      </c>
+      <c r="F69">
+        <v>3.4960354799137563</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>1.0947644252537633E-47</v>
+      </c>
+      <c r="B70">
+        <v>4.9303806576313238E-32</v>
+      </c>
+      <c r="C70">
+        <v>1.4791141972893971E-31</v>
+      </c>
+      <c r="D70">
+        <v>-4.9303806576313238E-32</v>
+      </c>
+      <c r="E70">
+        <v>4.2308444229492856</v>
+      </c>
+      <c r="F70">
+        <v>3.4350466320112143</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f>A65-A3</f>
+        <v>0</v>
+      </c>
+      <c r="B73">
+        <f t="shared" ref="B73:F73" si="22">B65-B3</f>
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" ref="A74:F74" si="23">A66-A4</f>
+        <v>0</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="23"/>
+        <v>-7.2164496600635175E-16</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" ref="A75:F75" si="24">A67-A5</f>
+        <v>0</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" ref="A76:F76" si="25">A68-A6</f>
+        <v>0</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <f t="shared" ref="A77:F77" si="26">A69-A7</f>
+        <v>-1.3684555315672042E-47</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="26"/>
+        <v>-9.8607613152626476E-32</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <f t="shared" ref="A78:F78" si="27">A70-A8</f>
+        <v>1.0947644252537633E-47</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="27"/>
+        <v>4.9303806576313238E-32</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="27"/>
+        <v>1.4791141972893971E-31</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="27"/>
+        <v>-4.9303806576313238E-32</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="27"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -10800,799 +12821,799 @@
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND()*10-3</f>
-        <v>6.717733902915608</v>
+        <v>5.9081057409099014</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:J16" ca="1" si="0">RAND()*10-3</f>
-        <v>3.5553225170189355</v>
+        <v>2.1612611726078992</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.3455434832802577</v>
+        <v>6.4624079813997106</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.86078111444708938</v>
+        <v>5.5573447470402471</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.5903986715303837</v>
+        <v>-2.0434637559353592</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9040799903836492</v>
+        <v>6.2009185330102756</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8713229854572599</v>
+        <v>-2.3221378800737229</v>
       </c>
       <c r="H1">
         <f ca="1">RAND()*10-3</f>
-        <v>5.537832619939886</v>
+        <v>-0.92201351434383216</v>
       </c>
       <c r="I1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.63129695795774587</v>
+        <v>1.997571181332563</v>
       </c>
       <c r="J1">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.5733219066366324</v>
+        <v>-0.26798845386909509</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:J19" ca="1" si="1">RAND()*10-3</f>
-        <v>5.3137142744978405</v>
+        <v>0.65671064040189542</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.294477673569528</v>
+        <v>-0.32375845526151181</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4284650425391998</v>
+        <v>5.0833925048767981</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8465890980057331</v>
+        <v>-2.7379735632965092</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2335883838376578</v>
+        <v>6.9986348703670949</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6627188467634024</v>
+        <v>-2.0188026042067539</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1009600613241171</v>
+        <v>5.0703581361773082</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2737636037967537</v>
+        <v>-2.674207719766208</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2836902568534114</v>
+        <v>2.0842728722494641</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>3.001569769448861</v>
+        <v>2.1532821674383902</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>6.9536270364633914</v>
+        <v>5.9795143305735294</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.5968446261309159</v>
+        <v>5.0645175423274331</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8960748893132369</v>
+        <v>-1.5605725001209476</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.0673425333504167</v>
+        <v>-1.8609779570043801</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1826979898131889</v>
+        <v>-2.6568600446963915</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.6641561561528735</v>
+        <v>2.8336879546248275</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.0877019907810319</v>
+        <v>0.43519700694061347</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2214449870976587</v>
+        <v>1.1920564271977367</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.0889545063244828</v>
+        <v>0.18043044386363993</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.6522655211059785</v>
+        <v>0.20371446168757323</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8810562379366971</v>
+        <v>-0.93943795212928682</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0037221664821736</v>
+        <v>-0.96599654671734569</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0065323508529804</v>
+        <v>5.7131829537656476</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>4.6340195465426239</v>
+        <v>2.0883775280424519</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.6911214632848663</v>
+        <v>5.2347277030088719</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0308740571306636</v>
+        <v>4.7273390451568194</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.6330784568443986</v>
+        <v>3.1350952632730662</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4944039459488518</v>
+        <v>-0.32166877436081087</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.6253598091942962</v>
+        <v>5.9315664817092451</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>5.3183566106361777</v>
+        <v>5.554666434024055</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2538499771743155</v>
+        <v>4.0648923425720884</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7598808172630589</v>
+        <v>2.2982072923555208</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5618873252537564</v>
+        <v>6.0882728150930028</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2853539759938233</v>
+        <v>4.1274934268792709</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7178395814641474</v>
+        <v>2.2727396804162581E-2</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6797305606328736</v>
+        <v>-2.6667643378465784</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5016905224139503</v>
+        <v>0.95758243999906778</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.5894509858853683</v>
+        <v>4.9187912407272529</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8385287211429029</v>
+        <v>6.0552463442125113</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97297641452823225</v>
+        <v>-1.5744921216397507</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.6891863306103978</v>
+        <v>0.18115839864061645</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7616151363010184</v>
+        <v>4.0078190083938132</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0460122683627002</v>
+        <v>-2.0672850150587325</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7295764589766325</v>
+        <v>0.78123775529854989</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>5.9178158193134518</v>
+        <v>-2.4201966465493445</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>5.3030144990120753</v>
+        <v>2.3509526623863319</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1736081553222206</v>
+        <v>4.040076215564552</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.36250522309819</v>
+        <v>-1.6286545298294703</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5437306038434482</v>
+        <v>-0.44060083802287853</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3416643298567088</v>
+        <v>-1.0473761338670247</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>1.8366844921083914</v>
+        <v>1.6639562964102863</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1813494037131793</v>
+        <v>0.49431562321701472</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1820481840969688</v>
+        <v>5.2910180659336543</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.5868431635874543</v>
+        <v>1.2620045542910407</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3020601367678912</v>
+        <v>-2.1414176939385761</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.1300883618037034</v>
+        <v>-0.4728941465156451</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.780069446922254</v>
+        <v>3.2437796622655366</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.81214151724536432</v>
+        <v>-1.8661635777454306</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45400281419021793</v>
+        <v>4.8023861591649091</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.5880682331540892</v>
+        <v>6.3858850591925922</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.76035307419624232</v>
+        <v>4.6180886460515538</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2173976928406356</v>
+        <v>0.71153968483897367</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.89275871457325096</v>
+        <v>-1.6640276760185064</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1602932024693251</v>
+        <v>6.5450522748421989</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5236388974069488</v>
+        <v>6.1398627679847593</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7818159806879521</v>
+        <v>-1.5618259996764656</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2789821412298643</v>
+        <v>1.6632678571434072</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2542062437996666</v>
+        <v>1.9742427507826807</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>6.306163192254477E-2</v>
+        <v>6.2741640715531322</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66240002413797594</v>
+        <v>0.19265128495879846</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24324202330469769</v>
+        <v>4.1593513147369672</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3920878756201445</v>
+        <v>3.8031950205103575</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66506802148368305</v>
+        <v>4.7965943520844423</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1877801519829809</v>
+        <v>-0.55091937004614078</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.621285304395343</v>
+        <v>1.7429469412787455</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8333481838934675</v>
+        <v>1.3785592487071838</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3984363750746889</v>
+        <v>-0.90766685305893002</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3890705034081581</v>
+        <v>-1.4831992671350553</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7480928081947171</v>
+        <v>6.1312264098936282</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4266623906207023</v>
+        <v>6.6367375836159823</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.34473787240880771</v>
+        <v>-0.76384802672699825</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2698154426710406</v>
+        <v>-0.33297151449601969</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2643073111939849</v>
+        <v>3.1889185064232883</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82700656596336763</v>
+        <v>9.3811227086098459E-2</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9940559680814758</v>
+        <v>5.4165060042823523</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5174985325126116</v>
+        <v>1.8697370633876789</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2345535092800031</v>
+        <v>3.4321381590986357</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5187355657756259</v>
+        <v>-2.8709057299960556</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4127521765245508</v>
+        <v>-0.36829737401550311</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4574456210990192</v>
+        <v>4.4233021833154105</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>6.007640936758893</v>
+        <v>-2.8680479312485438</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0835992689147602</v>
+        <v>0.64355827033708479</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7121644987271569</v>
+        <v>5.9829483466566522</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.38102901318748561</v>
+        <v>0.1525001827670307</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6893657165136569</v>
+        <v>2.6139114013314719</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9478479297333813</v>
+        <v>-2.5046268658116584</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.7472055384364955</v>
+        <v>6.0965085565553458</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.1699474711073461</v>
+        <v>-0.88423583108774828</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.81591119237525689</v>
+        <v>1.6105502200345372</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14990756408521255</v>
+        <v>-0.81087622156656636</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9867932581025514</v>
+        <v>5.2032838621444153</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7861361219643115</v>
+        <v>-0.53392972926633098</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3997084791563896</v>
+        <v>-0.76055116112362553</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8179978855963963</v>
+        <v>6.4347288256158599</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.010861103991024</v>
+        <v>1.4500584826679717</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4613444100927495</v>
+        <v>6.3791844848293291</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2504598834629626</v>
+        <v>2.5204189491877624</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.893443617138427</v>
+        <v>2.6798286517677186</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2089384784338275</v>
+        <v>0.58842957841969756</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0641249273154934</v>
+        <v>-2.1332205301175162</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.6839834709097627</v>
+        <v>6.5734416458711671</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.9551352228703196</v>
+        <v>1.0560403396861471</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.4144479885519829</v>
+        <v>2.3396484826704658</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0302544614307543</v>
+        <v>-2.8221729202083665</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0785845756642036</v>
+        <v>-1.3194020566945792</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.3021625131223065</v>
+        <v>5.6076922812385153</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1435956940663861</v>
+        <v>-0.30932590476013777</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37702803279760877</v>
+        <v>5.7158607908224539</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7824912068195875</v>
+        <v>-0.9869061259632943</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1283512241771794</v>
+        <v>2.0114530253532239</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4961313231808315</v>
+        <v>3.1624642080660985</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1031663552363753E-2</v>
+        <v>-2.1268587650119946</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.12066529961161176</v>
+        <v>3.657816504333514</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.0630563515512721</v>
+        <v>3.8059563987048923</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>3.087454144586701</v>
+        <v>-1.5451017642065952</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.6217260915621186</v>
+        <v>0.40685042508839597</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3505396256964062</v>
+        <v>-2.1272929294372096</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3651638311060275</v>
+        <v>-1.2175395000535822</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6771997975650521</v>
+        <v>0.75433951904400409</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.3914641011794233</v>
+        <v>6.6987947956252327</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.96294419472660309</v>
+        <v>3.2795953602541257</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1007552641653238</v>
+        <v>2.5514365001437866</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0170594345749437</v>
+        <v>4.3781345953332966</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7887512199059614</v>
+        <v>6.8717083334848112</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.2763833688339057</v>
+        <v>5.690677130126975</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0038409254847034</v>
+        <v>3.0843212209696436</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9727432226461605</v>
+        <v>3.3300870054673357</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.15564238009735654</v>
+        <v>-2.0196391452439606</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8404113503503083</v>
+        <v>-2.9004213596361312</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8447670278717716</v>
+        <v>2.696824578678223</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.6430100825285749</v>
+        <v>5.9169971877066754</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.0799363637658461</v>
+        <v>3.4712557363632222</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>5.3789803848314897</v>
+        <v>-2.2728648145259882</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.6061516092986523</v>
+        <v>3.3107352311025799</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.0255804668377184E-2</v>
+        <v>-0.98324228727079532</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2084740354851284</v>
+        <v>-1.0651121130536862</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4748010377564587</v>
+        <v>-2.7228769688256578</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8413444789528466</v>
+        <v>-1.7714754352823299</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9528298286323498</v>
+        <v>5.4348276410813448</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1396815459418743</v>
+        <v>-2.6226596242923423</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2950549620416938</v>
+        <v>6.5441097467067415</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4402409594023133</v>
+        <v>-0.22405831563400769</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.42052811480195995</v>
+        <v>-1.8339443444535637</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4198292496392995</v>
+        <v>-1.2846268285662872</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.57658876821743288</v>
+        <v>3.1852588155241772</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1902793609858424</v>
+        <v>1.9358564191418992</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>4.6302957182637012</v>
+        <v>0.74717734584096185</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>5.4145971051278199</v>
+        <v>6.5345000427962407</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.140469592384326</v>
+        <v>1.4357767263777408</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.5509540206006185</v>
+        <v>-6.808450664738519E-2</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8022148532747249</v>
+        <v>6.467901152371363</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>3.9222737306118862</v>
+        <v>-0.26705455110084886</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1459378315165925</v>
+        <v>4.6897537562110498</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.7060668564374721</v>
+        <v>-2.5877934910828824</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.9602658274143572</v>
+        <v>5.0052815725087765</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>4.1934235877943316E-2</v>
+        <v>1.7029414595378292</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.7698190123913764</v>
+        <v>-2.4789446996533853</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.61116467490598669</v>
+        <v>3.5121041393116066</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>6.2211754044852228</v>
+        <v>-1.8828270823832267</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6872778058184164</v>
+        <v>2.9558359661763056</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.91537782744292961</v>
+        <v>6.4180725381844805</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.7092609952710234E-3</v>
+        <v>5.6062743388246581</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7652051909896231</v>
+        <v>4.9856635322474467</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3604775475285997</v>
+        <v>4.5533454845564219</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>4.6738204169037028</v>
+        <v>3.1452105689259673</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>5.71125064013364</v>
+        <v>1.0142696507963116</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8524339832472556</v>
+        <v>3.2012003967220819</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8474680289882448</v>
+        <v>-1.2253873327789995</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0048596449991329</v>
+        <v>-2.8062718381977065</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.18399490132810348</v>
+        <v>2.9739367130726775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>